<commit_message>
Suporte a goal vindo do banco quando é alteração.
</commit_message>
<xml_diff>
--- a/doc/TemplatePlanilhaComProjetoDoUsuario.xlsx
+++ b/doc/TemplatePlanilhaComProjetoDoUsuario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\rurallegal\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE1867A-CCC0-4C19-8855-C999DC84DD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448109FD-1671-46CB-835C-5566E56FCF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="782" firstSheet="2" activeTab="9" xr2:uid="{C6048805-B876-472F-813A-7447540CBDCB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="782" firstSheet="2" activeTab="2" xr2:uid="{C6048805-B876-472F-813A-7447540CBDCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicas de Uso" sheetId="10" r:id="rId1"/>
@@ -3557,6 +3557,12 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3620,12 +3626,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3635,6 +3635,9 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="65">
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00;[Red]\-#,##0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -3946,9 +3949,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
@@ -53973,14 +53973,14 @@
     <dataField name="Sum of ValorEspFaixa" fld="20" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="14" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -54105,12 +54105,12 @@
       <calculatedColumnFormula>VLOOKUP(tbFcFaixa[[#This Row],[Faixa]],tbFaixa[],2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{0AABE378-5532-4D2F-BE0B-76BEBD410E33}" name="VTReceitas" dataDxfId="17">
-      <calculatedColumnFormula>SUMIFS(tbRec[ValorEspFaixa],tbRec[Faixa],tbFcFaixa[[#This Row],[Faixa]],tbRec[Idade],tbFcFaixa[[#This Row],[ano]])*tbFcFaixa[[#This Row],[Multiplicador]]*IF(tbFcFaixa[[#This Row],[ano]]&gt;=4,1*(1.5/tbFcFaixa[[#This Row],[ano]]),1)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUMIFS(tbRec[ValorEspFaixa],tbRec[Faixa],tbFcFaixa[[#This Row],[Faixa]],tbRec[Idade],tbFcFaixa[[#This Row],[ano]])*tbFcFaixa[[#This Row],[Multiplicador]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{5198B0B0-16AB-4E0C-A7AF-746C61E2A7BF}" name="VTCustos" dataDxfId="16">
       <calculatedColumnFormula>SUMIFS(tbResumo[ValorEspFaixa],tbResumo[Faixa],tbFcFaixa[[#This Row],[Faixa]],tbResumo[Ano],tbFcFaixa[[#This Row],[ano]])*tbFcFaixa[[#This Row],[Multiplicador]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{223E4A16-FBF0-4551-9B41-20351ACAC035}" name="VTLiquido" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="6" xr3:uid="{223E4A16-FBF0-4551-9B41-20351ACAC035}" name="VTLiquido" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="0">
       <calculatedColumnFormula>tbFcFaixa[[#This Row],[VTReceitas]]-tbFcFaixa[[#This Row],[VTCustos]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -54119,25 +54119,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8579E6BB-FC18-4413-BA32-A3626F0BC757}" name="tbDistribuicao" displayName="tbDistribuicao" ref="BU2:BY3" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11" headerRowCellStyle="Comma" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8579E6BB-FC18-4413-BA32-A3626F0BC757}" name="tbDistribuicao" displayName="tbDistribuicao" ref="BU2:BY3" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12" headerRowCellStyle="Comma" dataCellStyle="Comma">
   <autoFilter ref="BU2:BY3" xr:uid="{8579E6BB-FC18-4413-BA32-A3626F0BC757}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{97F0A431-E53A-4173-B7B6-4F327998E570}" name="Faixa" dataDxfId="10" dataCellStyle="Comma"/>
-    <tableColumn id="2" xr3:uid="{20805444-6442-4411-912E-85D698DAB74B}" name="Grupo" dataDxfId="9" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{65663903-6B14-441D-83C6-2B6C59DB8D0E}" name="Especie" dataDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{E5291598-5B87-4B9B-B2F0-7A1B65646F57}" name="NomeCientifico" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{DF6530C5-B271-4164-9526-8AD3E616095D}" name="NrArvores" dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{97F0A431-E53A-4173-B7B6-4F327998E570}" name="Faixa" dataDxfId="11" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{20805444-6442-4411-912E-85D698DAB74B}" name="Grupo" dataDxfId="10" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{65663903-6B14-441D-83C6-2B6C59DB8D0E}" name="Especie" dataDxfId="9" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{E5291598-5B87-4B9B-B2F0-7A1B65646F57}" name="NomeCientifico" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{DF6530C5-B271-4164-9526-8AD3E616095D}" name="NrArvores" dataDxfId="7" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DAC085FB-F3AD-424F-8809-C741E0F91E87}" name="tbUnid" displayName="tbUnid" ref="A1:B2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DAC085FB-F3AD-424F-8809-C741E0F91E87}" name="tbUnid" displayName="tbUnid" ref="A1:B2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:B2" xr:uid="{DAC085FB-F3AD-424F-8809-C741E0F91E87}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C44199EF-5CAF-41DE-AC50-9C8ADD924820}" name="Recurso" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{AF9227DF-33D6-480D-9CB7-FD60F7BC1811}" name="Unidade" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C44199EF-5CAF-41DE-AC50-9C8ADD924820}" name="Recurso" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{AF9227DF-33D6-480D-9CB7-FD60F7BC1811}" name="Unidade" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -57064,7 +57064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE23690A-A895-4002-97F8-748A1ADF99F4}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -58791,7 +58791,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58841,7 +58841,7 @@
         <v>#N/A</v>
       </c>
       <c r="E2" s="12" t="e">
-        <f>SUMIFS(tbRec[ValorEspFaixa],tbRec[Faixa],tbFcFaixa[[#This Row],[Faixa]],tbRec[Idade],tbFcFaixa[[#This Row],[ano]])*tbFcFaixa[[#This Row],[Multiplicador]]*IF(tbFcFaixa[[#This Row],[ano]]&gt;=4,1*(1.5/tbFcFaixa[[#This Row],[ano]]),1)</f>
+        <f>SUMIFS(tbRec[ValorEspFaixa],tbRec[Faixa],tbFcFaixa[[#This Row],[Faixa]],tbRec[Idade],tbFcFaixa[[#This Row],[ano]])*tbFcFaixa[[#This Row],[Multiplicador]]</f>
         <v>#N/A</v>
       </c>
       <c r="F2" s="12" t="e">
@@ -58897,27 +58897,27 @@
         <v>74</v>
       </c>
       <c r="B1" s="41" t="e">
-        <f>SUM(B3:B32)</f>
+        <f t="shared" ref="B1:G1" si="0">SUM(B3:B32)</f>
         <v>#N/A</v>
       </c>
       <c r="C1" s="41" t="e">
-        <f>SUM(C3:C32)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="D1" s="41" t="e">
-        <f>SUM(D3:D32)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E1" s="41" t="e">
-        <f>SUM(E3:E32)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F1" s="41" t="e">
-        <f>SUM(F3:F32)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="G1" s="41" t="e">
-        <f>SUM(G3:G32)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="H1" s="41" t="e">
@@ -59029,7 +59029,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="36">
-        <f t="shared" ref="G4:G32" si="0">E4-F4</f>
+        <f t="shared" ref="G4:G32" si="1">E4-F4</f>
         <v>0</v>
       </c>
       <c r="H4" s="37" t="e">
@@ -59077,11 +59077,11 @@
         <v>0</v>
       </c>
       <c r="G5" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5" s="37" t="e">
-        <f t="shared" ref="H5:H32" si="1">H4+D5</f>
+        <f t="shared" ref="H5:H32" si="2">H4+D5</f>
         <v>#N/A</v>
       </c>
       <c r="I5" s="18" t="e">
@@ -59125,11 +59125,11 @@
         <v>0</v>
       </c>
       <c r="G6" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I6" s="18" t="e">
@@ -59177,15 +59177,15 @@
         <v>0</v>
       </c>
       <c r="G7" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H7" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I7" s="18" t="e">
-        <f t="shared" ref="I7:I32" si="2">I6*(1+$M$8)</f>
+        <f t="shared" ref="I7:I32" si="3">I6*(1+$M$8)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -59214,21 +59214,21 @@
         <v>0</v>
       </c>
       <c r="G8" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H8" s="37" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I8" s="18" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="K8" s="182" t="s">
+      <c r="I8" s="18" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K8" s="161" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="183"/>
+      <c r="L8" s="162"/>
       <c r="M8" s="32">
         <v>7.8899999999999998E-2</v>
       </c>
@@ -59259,15 +59259,15 @@
         <v>0</v>
       </c>
       <c r="G9" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H9" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I9" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59296,15 +59296,15 @@
         <v>0</v>
       </c>
       <c r="G10" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H10" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I10" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59333,15 +59333,15 @@
         <v>0</v>
       </c>
       <c r="G11" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H11" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I11" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59370,15 +59370,15 @@
         <v>0</v>
       </c>
       <c r="G12" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H12" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I12" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59407,15 +59407,15 @@
         <v>0</v>
       </c>
       <c r="G13" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H13" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I13" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59444,15 +59444,15 @@
         <v>0</v>
       </c>
       <c r="G14" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H14" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I14" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59481,15 +59481,15 @@
         <v>0</v>
       </c>
       <c r="G15" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H15" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I15" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59518,15 +59518,15 @@
         <v>0</v>
       </c>
       <c r="G16" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H16" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I16" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59555,15 +59555,15 @@
         <v>0</v>
       </c>
       <c r="G17" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H17" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I17" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59592,15 +59592,15 @@
         <v>0</v>
       </c>
       <c r="G18" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H18" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I18" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59629,15 +59629,15 @@
         <v>0</v>
       </c>
       <c r="G19" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H19" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I19" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59666,15 +59666,15 @@
         <v>0</v>
       </c>
       <c r="G20" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H20" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I20" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59703,15 +59703,15 @@
         <v>0</v>
       </c>
       <c r="G21" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I21" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59740,15 +59740,15 @@
         <v>0</v>
       </c>
       <c r="G22" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H22" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I22" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59777,15 +59777,15 @@
         <v>0</v>
       </c>
       <c r="G23" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H23" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I23" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59814,15 +59814,15 @@
         <v>0</v>
       </c>
       <c r="G24" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H24" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I24" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59851,15 +59851,15 @@
         <v>0</v>
       </c>
       <c r="G25" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H25" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I25" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59888,15 +59888,15 @@
         <v>0</v>
       </c>
       <c r="G26" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H26" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I26" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59925,15 +59925,15 @@
         <v>0</v>
       </c>
       <c r="G27" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H27" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I27" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59962,15 +59962,15 @@
         <v>0</v>
       </c>
       <c r="G28" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H28" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I28" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -59999,15 +59999,15 @@
         <v>0</v>
       </c>
       <c r="G29" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H29" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I29" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -60036,15 +60036,15 @@
         <v>0</v>
       </c>
       <c r="G30" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H30" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I30" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -60073,15 +60073,15 @@
         <v>0</v>
       </c>
       <c r="G31" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H31" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I31" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -60110,15 +60110,15 @@
         <v>0</v>
       </c>
       <c r="G32" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H32" s="37" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I32" s="18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -60135,7 +60135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10EA992-D83A-4210-ACEC-3D751E1F72C2}">
   <dimension ref="B1:CZ46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BS1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="BS1" workbookViewId="0">
       <selection activeCell="BU3" sqref="BU3"/>
     </sheetView>
   </sheetViews>
@@ -60154,84 +60154,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:104" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="177" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
-      <c r="AD1" s="176"/>
-      <c r="AE1" s="176"/>
-      <c r="AF1" s="176"/>
-      <c r="AG1" s="176"/>
-      <c r="AH1" s="176"/>
-      <c r="AI1" s="176"/>
-      <c r="AJ1" s="177"/>
-      <c r="AN1" s="161" t="s">
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
+      <c r="P1" s="178"/>
+      <c r="Q1" s="178"/>
+      <c r="R1" s="178"/>
+      <c r="S1" s="178"/>
+      <c r="T1" s="178"/>
+      <c r="U1" s="178"/>
+      <c r="V1" s="178"/>
+      <c r="W1" s="178"/>
+      <c r="X1" s="178"/>
+      <c r="Y1" s="178"/>
+      <c r="Z1" s="178"/>
+      <c r="AA1" s="178"/>
+      <c r="AB1" s="178"/>
+      <c r="AC1" s="178"/>
+      <c r="AD1" s="178"/>
+      <c r="AE1" s="178"/>
+      <c r="AF1" s="178"/>
+      <c r="AG1" s="178"/>
+      <c r="AH1" s="178"/>
+      <c r="AI1" s="178"/>
+      <c r="AJ1" s="179"/>
+      <c r="AN1" s="163" t="s">
         <v>335</v>
       </c>
-      <c r="AO1" s="162"/>
-      <c r="AP1" s="162"/>
-      <c r="AQ1" s="162"/>
-      <c r="AR1" s="162"/>
-      <c r="AS1" s="162"/>
-      <c r="AT1" s="162"/>
-      <c r="AU1" s="162"/>
-      <c r="AV1" s="162"/>
-      <c r="AW1" s="162"/>
-      <c r="AX1" s="162"/>
-      <c r="AY1" s="162"/>
-      <c r="AZ1" s="162"/>
-      <c r="BA1" s="162"/>
-      <c r="BB1" s="162"/>
-      <c r="BC1" s="162"/>
-      <c r="BD1" s="162"/>
-      <c r="BE1" s="162"/>
-      <c r="BF1" s="162"/>
-      <c r="BG1" s="162"/>
-      <c r="BH1" s="162"/>
-      <c r="BI1" s="162"/>
-      <c r="BJ1" s="162"/>
-      <c r="BK1" s="162"/>
-      <c r="BL1" s="162"/>
-      <c r="BM1" s="162"/>
-      <c r="BN1" s="162"/>
-      <c r="BO1" s="162"/>
-      <c r="BP1" s="162"/>
-      <c r="BQ1" s="162"/>
-      <c r="BR1" s="162"/>
-      <c r="BS1" s="163"/>
-      <c r="BU1" s="164" t="s">
+      <c r="AO1" s="164"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
+      <c r="AS1" s="164"/>
+      <c r="AT1" s="164"/>
+      <c r="AU1" s="164"/>
+      <c r="AV1" s="164"/>
+      <c r="AW1" s="164"/>
+      <c r="AX1" s="164"/>
+      <c r="AY1" s="164"/>
+      <c r="AZ1" s="164"/>
+      <c r="BA1" s="164"/>
+      <c r="BB1" s="164"/>
+      <c r="BC1" s="164"/>
+      <c r="BD1" s="164"/>
+      <c r="BE1" s="164"/>
+      <c r="BF1" s="164"/>
+      <c r="BG1" s="164"/>
+      <c r="BH1" s="164"/>
+      <c r="BI1" s="164"/>
+      <c r="BJ1" s="164"/>
+      <c r="BK1" s="164"/>
+      <c r="BL1" s="164"/>
+      <c r="BM1" s="164"/>
+      <c r="BN1" s="164"/>
+      <c r="BO1" s="164"/>
+      <c r="BP1" s="164"/>
+      <c r="BQ1" s="164"/>
+      <c r="BR1" s="164"/>
+      <c r="BS1" s="165"/>
+      <c r="BU1" s="166" t="s">
         <v>336</v>
       </c>
-      <c r="BV1" s="165"/>
-      <c r="BW1" s="165"/>
-      <c r="BX1" s="165"/>
-      <c r="BY1" s="165"/>
+      <c r="BV1" s="167"/>
+      <c r="BW1" s="167"/>
+      <c r="BX1" s="167"/>
+      <c r="BY1" s="167"/>
       <c r="BZ1" s="112"/>
       <c r="CA1" s="112"/>
       <c r="CB1" s="112"/>
@@ -60261,41 +60261,41 @@
       <c r="CZ1" s="113"/>
     </row>
     <row r="2" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B2" s="178"/>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179"/>
-      <c r="I2" s="179"/>
-      <c r="J2" s="179"/>
-      <c r="K2" s="179"/>
-      <c r="L2" s="179"/>
-      <c r="M2" s="179"/>
-      <c r="N2" s="179"/>
-      <c r="O2" s="179"/>
-      <c r="P2" s="179"/>
-      <c r="Q2" s="179"/>
-      <c r="R2" s="179"/>
-      <c r="S2" s="179"/>
-      <c r="T2" s="179"/>
-      <c r="U2" s="179"/>
-      <c r="V2" s="179"/>
-      <c r="W2" s="179"/>
-      <c r="X2" s="179"/>
-      <c r="Y2" s="179"/>
-      <c r="Z2" s="179"/>
-      <c r="AA2" s="179"/>
-      <c r="AB2" s="179"/>
-      <c r="AC2" s="179"/>
-      <c r="AD2" s="179"/>
-      <c r="AE2" s="179"/>
-      <c r="AF2" s="179"/>
-      <c r="AG2" s="179"/>
-      <c r="AH2" s="179"/>
-      <c r="AI2" s="179"/>
-      <c r="AJ2" s="180"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="181"/>
+      <c r="H2" s="181"/>
+      <c r="I2" s="181"/>
+      <c r="J2" s="181"/>
+      <c r="K2" s="181"/>
+      <c r="L2" s="181"/>
+      <c r="M2" s="181"/>
+      <c r="N2" s="181"/>
+      <c r="O2" s="181"/>
+      <c r="P2" s="181"/>
+      <c r="Q2" s="181"/>
+      <c r="R2" s="181"/>
+      <c r="S2" s="181"/>
+      <c r="T2" s="181"/>
+      <c r="U2" s="181"/>
+      <c r="V2" s="181"/>
+      <c r="W2" s="181"/>
+      <c r="X2" s="181"/>
+      <c r="Y2" s="181"/>
+      <c r="Z2" s="181"/>
+      <c r="AA2" s="181"/>
+      <c r="AB2" s="181"/>
+      <c r="AC2" s="181"/>
+      <c r="AD2" s="181"/>
+      <c r="AE2" s="181"/>
+      <c r="AF2" s="181"/>
+      <c r="AG2" s="181"/>
+      <c r="AH2" s="181"/>
+      <c r="AI2" s="181"/>
+      <c r="AJ2" s="182"/>
       <c r="AN2" s="103" t="s">
         <v>271</v>
       </c>
@@ -60438,43 +60438,43 @@
       </c>
     </row>
     <row r="4" spans="2:104" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="166" t="s">
+      <c r="B4" s="168" t="s">
         <v>303</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
-      <c r="H4" s="167"/>
-      <c r="I4" s="167"/>
-      <c r="J4" s="167"/>
-      <c r="K4" s="167"/>
-      <c r="L4" s="167"/>
-      <c r="M4" s="167"/>
-      <c r="N4" s="167"/>
-      <c r="O4" s="167"/>
-      <c r="P4" s="167"/>
-      <c r="Q4" s="167"/>
-      <c r="R4" s="167"/>
-      <c r="S4" s="167"/>
-      <c r="T4" s="167"/>
-      <c r="U4" s="167"/>
-      <c r="V4" s="167"/>
-      <c r="W4" s="167"/>
-      <c r="X4" s="167"/>
-      <c r="Y4" s="167"/>
-      <c r="Z4" s="167"/>
-      <c r="AA4" s="167"/>
-      <c r="AB4" s="167"/>
-      <c r="AC4" s="167"/>
-      <c r="AD4" s="167"/>
-      <c r="AE4" s="167"/>
-      <c r="AF4" s="167"/>
-      <c r="AG4" s="167"/>
-      <c r="AH4" s="167"/>
-      <c r="AI4" s="167"/>
-      <c r="AJ4" s="168"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
+      <c r="F4" s="169"/>
+      <c r="G4" s="169"/>
+      <c r="H4" s="169"/>
+      <c r="I4" s="169"/>
+      <c r="J4" s="169"/>
+      <c r="K4" s="169"/>
+      <c r="L4" s="169"/>
+      <c r="M4" s="169"/>
+      <c r="N4" s="169"/>
+      <c r="O4" s="169"/>
+      <c r="P4" s="169"/>
+      <c r="Q4" s="169"/>
+      <c r="R4" s="169"/>
+      <c r="S4" s="169"/>
+      <c r="T4" s="169"/>
+      <c r="U4" s="169"/>
+      <c r="V4" s="169"/>
+      <c r="W4" s="169"/>
+      <c r="X4" s="169"/>
+      <c r="Y4" s="169"/>
+      <c r="Z4" s="169"/>
+      <c r="AA4" s="169"/>
+      <c r="AB4" s="169"/>
+      <c r="AC4" s="169"/>
+      <c r="AD4" s="169"/>
+      <c r="AE4" s="169"/>
+      <c r="AF4" s="169"/>
+      <c r="AG4" s="169"/>
+      <c r="AH4" s="169"/>
+      <c r="AI4" s="169"/>
+      <c r="AJ4" s="170"/>
       <c r="AN4" s="107" t="s">
         <v>276</v>
       </c>
@@ -60515,41 +60515,41 @@
       <c r="BS4" s="106"/>
     </row>
     <row r="5" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B5" s="169"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="170"/>
-      <c r="K5" s="170"/>
-      <c r="L5" s="170"/>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="170"/>
-      <c r="Q5" s="170"/>
-      <c r="R5" s="170"/>
-      <c r="S5" s="170"/>
-      <c r="T5" s="170"/>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="170"/>
-      <c r="Y5" s="170"/>
-      <c r="Z5" s="170"/>
-      <c r="AA5" s="170"/>
-      <c r="AB5" s="170"/>
-      <c r="AC5" s="170"/>
-      <c r="AD5" s="170"/>
-      <c r="AE5" s="170"/>
-      <c r="AF5" s="170"/>
-      <c r="AG5" s="170"/>
-      <c r="AH5" s="170"/>
-      <c r="AI5" s="170"/>
-      <c r="AJ5" s="171"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="172"/>
+      <c r="I5" s="172"/>
+      <c r="J5" s="172"/>
+      <c r="K5" s="172"/>
+      <c r="L5" s="172"/>
+      <c r="M5" s="172"/>
+      <c r="N5" s="172"/>
+      <c r="O5" s="172"/>
+      <c r="P5" s="172"/>
+      <c r="Q5" s="172"/>
+      <c r="R5" s="172"/>
+      <c r="S5" s="172"/>
+      <c r="T5" s="172"/>
+      <c r="U5" s="172"/>
+      <c r="V5" s="172"/>
+      <c r="W5" s="172"/>
+      <c r="X5" s="172"/>
+      <c r="Y5" s="172"/>
+      <c r="Z5" s="172"/>
+      <c r="AA5" s="172"/>
+      <c r="AB5" s="172"/>
+      <c r="AC5" s="172"/>
+      <c r="AD5" s="172"/>
+      <c r="AE5" s="172"/>
+      <c r="AF5" s="172"/>
+      <c r="AG5" s="172"/>
+      <c r="AH5" s="172"/>
+      <c r="AI5" s="172"/>
+      <c r="AJ5" s="173"/>
       <c r="AN5" s="108" t="s">
         <v>280</v>
       </c>
@@ -60590,157 +60590,157 @@
       <c r="BS5" s="111"/>
     </row>
     <row r="6" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B6" s="169"/>
-      <c r="C6" s="170"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="170"/>
-      <c r="H6" s="170"/>
-      <c r="I6" s="170"/>
-      <c r="J6" s="170"/>
-      <c r="K6" s="170"/>
-      <c r="L6" s="170"/>
-      <c r="M6" s="170"/>
-      <c r="N6" s="170"/>
-      <c r="O6" s="170"/>
-      <c r="P6" s="170"/>
-      <c r="Q6" s="170"/>
-      <c r="R6" s="170"/>
-      <c r="S6" s="170"/>
-      <c r="T6" s="170"/>
-      <c r="U6" s="170"/>
-      <c r="V6" s="170"/>
-      <c r="W6" s="170"/>
-      <c r="X6" s="170"/>
-      <c r="Y6" s="170"/>
-      <c r="Z6" s="170"/>
-      <c r="AA6" s="170"/>
-      <c r="AB6" s="170"/>
-      <c r="AC6" s="170"/>
-      <c r="AD6" s="170"/>
-      <c r="AE6" s="170"/>
-      <c r="AF6" s="170"/>
-      <c r="AG6" s="170"/>
-      <c r="AH6" s="170"/>
-      <c r="AI6" s="170"/>
-      <c r="AJ6" s="171"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="172"/>
+      <c r="H6" s="172"/>
+      <c r="I6" s="172"/>
+      <c r="J6" s="172"/>
+      <c r="K6" s="172"/>
+      <c r="L6" s="172"/>
+      <c r="M6" s="172"/>
+      <c r="N6" s="172"/>
+      <c r="O6" s="172"/>
+      <c r="P6" s="172"/>
+      <c r="Q6" s="172"/>
+      <c r="R6" s="172"/>
+      <c r="S6" s="172"/>
+      <c r="T6" s="172"/>
+      <c r="U6" s="172"/>
+      <c r="V6" s="172"/>
+      <c r="W6" s="172"/>
+      <c r="X6" s="172"/>
+      <c r="Y6" s="172"/>
+      <c r="Z6" s="172"/>
+      <c r="AA6" s="172"/>
+      <c r="AB6" s="172"/>
+      <c r="AC6" s="172"/>
+      <c r="AD6" s="172"/>
+      <c r="AE6" s="172"/>
+      <c r="AF6" s="172"/>
+      <c r="AG6" s="172"/>
+      <c r="AH6" s="172"/>
+      <c r="AI6" s="172"/>
+      <c r="AJ6" s="173"/>
       <c r="AM6" s="86"/>
       <c r="BS6"/>
     </row>
     <row r="7" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B7" s="169"/>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="170"/>
-      <c r="H7" s="170"/>
-      <c r="I7" s="170"/>
-      <c r="J7" s="170"/>
-      <c r="K7" s="170"/>
-      <c r="L7" s="170"/>
-      <c r="M7" s="170"/>
-      <c r="N7" s="170"/>
-      <c r="O7" s="170"/>
-      <c r="P7" s="170"/>
-      <c r="Q7" s="170"/>
-      <c r="R7" s="170"/>
-      <c r="S7" s="170"/>
-      <c r="T7" s="170"/>
-      <c r="U7" s="170"/>
-      <c r="V7" s="170"/>
-      <c r="W7" s="170"/>
-      <c r="X7" s="170"/>
-      <c r="Y7" s="170"/>
-      <c r="Z7" s="170"/>
-      <c r="AA7" s="170"/>
-      <c r="AB7" s="170"/>
-      <c r="AC7" s="170"/>
-      <c r="AD7" s="170"/>
-      <c r="AE7" s="170"/>
-      <c r="AF7" s="170"/>
-      <c r="AG7" s="170"/>
-      <c r="AH7" s="170"/>
-      <c r="AI7" s="170"/>
-      <c r="AJ7" s="171"/>
-      <c r="AN7" s="181" t="s">
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="172"/>
+      <c r="H7" s="172"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="172"/>
+      <c r="K7" s="172"/>
+      <c r="L7" s="172"/>
+      <c r="M7" s="172"/>
+      <c r="N7" s="172"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="172"/>
+      <c r="Q7" s="172"/>
+      <c r="R7" s="172"/>
+      <c r="S7" s="172"/>
+      <c r="T7" s="172"/>
+      <c r="U7" s="172"/>
+      <c r="V7" s="172"/>
+      <c r="W7" s="172"/>
+      <c r="X7" s="172"/>
+      <c r="Y7" s="172"/>
+      <c r="Z7" s="172"/>
+      <c r="AA7" s="172"/>
+      <c r="AB7" s="172"/>
+      <c r="AC7" s="172"/>
+      <c r="AD7" s="172"/>
+      <c r="AE7" s="172"/>
+      <c r="AF7" s="172"/>
+      <c r="AG7" s="172"/>
+      <c r="AH7" s="172"/>
+      <c r="AI7" s="172"/>
+      <c r="AJ7" s="173"/>
+      <c r="AN7" s="183" t="s">
         <v>278</v>
       </c>
-      <c r="AO7" s="181"/>
-      <c r="AP7" s="181"/>
-      <c r="AQ7" s="181"/>
-      <c r="AR7" s="181"/>
-      <c r="AS7" s="181"/>
-      <c r="AT7" s="181"/>
-      <c r="AU7" s="181"/>
-      <c r="AV7" s="181" t="s">
+      <c r="AO7" s="183"/>
+      <c r="AP7" s="183"/>
+      <c r="AQ7" s="183"/>
+      <c r="AR7" s="183"/>
+      <c r="AS7" s="183"/>
+      <c r="AT7" s="183"/>
+      <c r="AU7" s="183"/>
+      <c r="AV7" s="183" t="s">
         <v>279</v>
       </c>
-      <c r="AW7" s="181"/>
-      <c r="AX7" s="181"/>
-      <c r="AY7" s="181"/>
-      <c r="AZ7" s="181"/>
-      <c r="BA7" s="181"/>
-      <c r="BB7" s="181"/>
-      <c r="BC7" s="181"/>
-      <c r="BD7" s="181" t="s">
+      <c r="AW7" s="183"/>
+      <c r="AX7" s="183"/>
+      <c r="AY7" s="183"/>
+      <c r="AZ7" s="183"/>
+      <c r="BA7" s="183"/>
+      <c r="BB7" s="183"/>
+      <c r="BC7" s="183"/>
+      <c r="BD7" s="183" t="s">
         <v>278</v>
       </c>
-      <c r="BE7" s="181"/>
-      <c r="BF7" s="181"/>
-      <c r="BG7" s="181"/>
-      <c r="BH7" s="181"/>
-      <c r="BI7" s="181"/>
-      <c r="BJ7" s="181"/>
-      <c r="BK7" s="181"/>
-      <c r="BL7" s="181" t="s">
+      <c r="BE7" s="183"/>
+      <c r="BF7" s="183"/>
+      <c r="BG7" s="183"/>
+      <c r="BH7" s="183"/>
+      <c r="BI7" s="183"/>
+      <c r="BJ7" s="183"/>
+      <c r="BK7" s="183"/>
+      <c r="BL7" s="183" t="s">
         <v>279</v>
       </c>
-      <c r="BM7" s="181"/>
-      <c r="BN7" s="181"/>
-      <c r="BO7" s="181"/>
-      <c r="BP7" s="181"/>
-      <c r="BQ7" s="181"/>
-      <c r="BR7" s="181"/>
-      <c r="BS7" s="181"/>
+      <c r="BM7" s="183"/>
+      <c r="BN7" s="183"/>
+      <c r="BO7" s="183"/>
+      <c r="BP7" s="183"/>
+      <c r="BQ7" s="183"/>
+      <c r="BR7" s="183"/>
+      <c r="BS7" s="183"/>
     </row>
     <row r="8" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B8" s="169"/>
-      <c r="C8" s="170"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="170"/>
-      <c r="G8" s="170"/>
-      <c r="H8" s="170"/>
-      <c r="I8" s="170"/>
-      <c r="J8" s="170"/>
-      <c r="K8" s="170"/>
-      <c r="L8" s="170"/>
-      <c r="M8" s="170"/>
-      <c r="N8" s="170"/>
-      <c r="O8" s="170"/>
-      <c r="P8" s="170"/>
-      <c r="Q8" s="170"/>
-      <c r="R8" s="170"/>
-      <c r="S8" s="170"/>
-      <c r="T8" s="170"/>
-      <c r="U8" s="170"/>
-      <c r="V8" s="170"/>
-      <c r="W8" s="170"/>
-      <c r="X8" s="170"/>
-      <c r="Y8" s="170"/>
-      <c r="Z8" s="170"/>
-      <c r="AA8" s="170"/>
-      <c r="AB8" s="170"/>
-      <c r="AC8" s="170"/>
-      <c r="AD8" s="170"/>
-      <c r="AE8" s="170"/>
-      <c r="AF8" s="170"/>
-      <c r="AG8" s="170"/>
-      <c r="AH8" s="170"/>
-      <c r="AI8" s="170"/>
-      <c r="AJ8" s="171"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="172"/>
+      <c r="H8" s="172"/>
+      <c r="I8" s="172"/>
+      <c r="J8" s="172"/>
+      <c r="K8" s="172"/>
+      <c r="L8" s="172"/>
+      <c r="M8" s="172"/>
+      <c r="N8" s="172"/>
+      <c r="O8" s="172"/>
+      <c r="P8" s="172"/>
+      <c r="Q8" s="172"/>
+      <c r="R8" s="172"/>
+      <c r="S8" s="172"/>
+      <c r="T8" s="172"/>
+      <c r="U8" s="172"/>
+      <c r="V8" s="172"/>
+      <c r="W8" s="172"/>
+      <c r="X8" s="172"/>
+      <c r="Y8" s="172"/>
+      <c r="Z8" s="172"/>
+      <c r="AA8" s="172"/>
+      <c r="AB8" s="172"/>
+      <c r="AC8" s="172"/>
+      <c r="AD8" s="172"/>
+      <c r="AE8" s="172"/>
+      <c r="AF8" s="172"/>
+      <c r="AG8" s="172"/>
+      <c r="AH8" s="172"/>
+      <c r="AI8" s="172"/>
+      <c r="AJ8" s="173"/>
       <c r="AN8" s="128">
         <v>1</v>
       </c>
@@ -60839,78 +60839,78 @@
       </c>
     </row>
     <row r="9" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B9" s="169"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="170"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="170"/>
-      <c r="K9" s="170"/>
-      <c r="L9" s="170"/>
-      <c r="M9" s="170"/>
-      <c r="N9" s="170"/>
-      <c r="O9" s="170"/>
-      <c r="P9" s="170"/>
-      <c r="Q9" s="170"/>
-      <c r="R9" s="170"/>
-      <c r="S9" s="170"/>
-      <c r="T9" s="170"/>
-      <c r="U9" s="170"/>
-      <c r="V9" s="170"/>
-      <c r="W9" s="170"/>
-      <c r="X9" s="170"/>
-      <c r="Y9" s="170"/>
-      <c r="Z9" s="170"/>
-      <c r="AA9" s="170"/>
-      <c r="AB9" s="170"/>
-      <c r="AC9" s="170"/>
-      <c r="AD9" s="170"/>
-      <c r="AE9" s="170"/>
-      <c r="AF9" s="170"/>
-      <c r="AG9" s="170"/>
-      <c r="AH9" s="170"/>
-      <c r="AI9" s="170"/>
-      <c r="AJ9" s="171"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="172"/>
+      <c r="H9" s="172"/>
+      <c r="I9" s="172"/>
+      <c r="J9" s="172"/>
+      <c r="K9" s="172"/>
+      <c r="L9" s="172"/>
+      <c r="M9" s="172"/>
+      <c r="N9" s="172"/>
+      <c r="O9" s="172"/>
+      <c r="P9" s="172"/>
+      <c r="Q9" s="172"/>
+      <c r="R9" s="172"/>
+      <c r="S9" s="172"/>
+      <c r="T9" s="172"/>
+      <c r="U9" s="172"/>
+      <c r="V9" s="172"/>
+      <c r="W9" s="172"/>
+      <c r="X9" s="172"/>
+      <c r="Y9" s="172"/>
+      <c r="Z9" s="172"/>
+      <c r="AA9" s="172"/>
+      <c r="AB9" s="172"/>
+      <c r="AC9" s="172"/>
+      <c r="AD9" s="172"/>
+      <c r="AE9" s="172"/>
+      <c r="AF9" s="172"/>
+      <c r="AG9" s="172"/>
+      <c r="AH9" s="172"/>
+      <c r="AI9" s="172"/>
+      <c r="AJ9" s="173"/>
     </row>
     <row r="10" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="170"/>
-      <c r="H10" s="170"/>
-      <c r="I10" s="170"/>
-      <c r="J10" s="170"/>
-      <c r="K10" s="170"/>
-      <c r="L10" s="170"/>
-      <c r="M10" s="170"/>
-      <c r="N10" s="170"/>
-      <c r="O10" s="170"/>
-      <c r="P10" s="170"/>
-      <c r="Q10" s="170"/>
-      <c r="R10" s="170"/>
-      <c r="S10" s="170"/>
-      <c r="T10" s="170"/>
-      <c r="U10" s="170"/>
-      <c r="V10" s="170"/>
-      <c r="W10" s="170"/>
-      <c r="X10" s="170"/>
-      <c r="Y10" s="170"/>
-      <c r="Z10" s="170"/>
-      <c r="AA10" s="170"/>
-      <c r="AB10" s="170"/>
-      <c r="AC10" s="170"/>
-      <c r="AD10" s="170"/>
-      <c r="AE10" s="170"/>
-      <c r="AF10" s="170"/>
-      <c r="AG10" s="170"/>
-      <c r="AH10" s="170"/>
-      <c r="AI10" s="170"/>
-      <c r="AJ10" s="171"/>
+      <c r="B10" s="171"/>
+      <c r="C10" s="172"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="172"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="172"/>
+      <c r="K10" s="172"/>
+      <c r="L10" s="172"/>
+      <c r="M10" s="172"/>
+      <c r="N10" s="172"/>
+      <c r="O10" s="172"/>
+      <c r="P10" s="172"/>
+      <c r="Q10" s="172"/>
+      <c r="R10" s="172"/>
+      <c r="S10" s="172"/>
+      <c r="T10" s="172"/>
+      <c r="U10" s="172"/>
+      <c r="V10" s="172"/>
+      <c r="W10" s="172"/>
+      <c r="X10" s="172"/>
+      <c r="Y10" s="172"/>
+      <c r="Z10" s="172"/>
+      <c r="AA10" s="172"/>
+      <c r="AB10" s="172"/>
+      <c r="AC10" s="172"/>
+      <c r="AD10" s="172"/>
+      <c r="AE10" s="172"/>
+      <c r="AF10" s="172"/>
+      <c r="AG10" s="172"/>
+      <c r="AH10" s="172"/>
+      <c r="AI10" s="172"/>
+      <c r="AJ10" s="173"/>
       <c r="AL10" s="149">
         <v>1</v>
       </c>
@@ -61012,41 +61012,41 @@
       </c>
     </row>
     <row r="11" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B11" s="169"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="170"/>
-      <c r="E11" s="170"/>
-      <c r="F11" s="170"/>
-      <c r="G11" s="170"/>
-      <c r="H11" s="170"/>
-      <c r="I11" s="170"/>
-      <c r="J11" s="170"/>
-      <c r="K11" s="170"/>
-      <c r="L11" s="170"/>
-      <c r="M11" s="170"/>
-      <c r="N11" s="170"/>
-      <c r="O11" s="170"/>
-      <c r="P11" s="170"/>
-      <c r="Q11" s="170"/>
-      <c r="R11" s="170"/>
-      <c r="S11" s="170"/>
-      <c r="T11" s="170"/>
-      <c r="U11" s="170"/>
-      <c r="V11" s="170"/>
-      <c r="W11" s="170"/>
-      <c r="X11" s="170"/>
-      <c r="Y11" s="170"/>
-      <c r="Z11" s="170"/>
-      <c r="AA11" s="170"/>
-      <c r="AB11" s="170"/>
-      <c r="AC11" s="170"/>
-      <c r="AD11" s="170"/>
-      <c r="AE11" s="170"/>
-      <c r="AF11" s="170"/>
-      <c r="AG11" s="170"/>
-      <c r="AH11" s="170"/>
-      <c r="AI11" s="170"/>
-      <c r="AJ11" s="171"/>
+      <c r="B11" s="171"/>
+      <c r="C11" s="172"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="172"/>
+      <c r="F11" s="172"/>
+      <c r="G11" s="172"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="172"/>
+      <c r="J11" s="172"/>
+      <c r="K11" s="172"/>
+      <c r="L11" s="172"/>
+      <c r="M11" s="172"/>
+      <c r="N11" s="172"/>
+      <c r="O11" s="172"/>
+      <c r="P11" s="172"/>
+      <c r="Q11" s="172"/>
+      <c r="R11" s="172"/>
+      <c r="S11" s="172"/>
+      <c r="T11" s="172"/>
+      <c r="U11" s="172"/>
+      <c r="V11" s="172"/>
+      <c r="W11" s="172"/>
+      <c r="X11" s="172"/>
+      <c r="Y11" s="172"/>
+      <c r="Z11" s="172"/>
+      <c r="AA11" s="172"/>
+      <c r="AB11" s="172"/>
+      <c r="AC11" s="172"/>
+      <c r="AD11" s="172"/>
+      <c r="AE11" s="172"/>
+      <c r="AF11" s="172"/>
+      <c r="AG11" s="172"/>
+      <c r="AH11" s="172"/>
+      <c r="AI11" s="172"/>
+      <c r="AJ11" s="173"/>
       <c r="AL11" s="150">
         <v>2</v>
       </c>
@@ -61148,41 +61148,41 @@
       </c>
     </row>
     <row r="12" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B12" s="169"/>
-      <c r="C12" s="170"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="170"/>
-      <c r="F12" s="170"/>
-      <c r="G12" s="170"/>
-      <c r="H12" s="170"/>
-      <c r="I12" s="170"/>
-      <c r="J12" s="170"/>
-      <c r="K12" s="170"/>
-      <c r="L12" s="170"/>
-      <c r="M12" s="170"/>
-      <c r="N12" s="170"/>
-      <c r="O12" s="170"/>
-      <c r="P12" s="170"/>
-      <c r="Q12" s="170"/>
-      <c r="R12" s="170"/>
-      <c r="S12" s="170"/>
-      <c r="T12" s="170"/>
-      <c r="U12" s="170"/>
-      <c r="V12" s="170"/>
-      <c r="W12" s="170"/>
-      <c r="X12" s="170"/>
-      <c r="Y12" s="170"/>
-      <c r="Z12" s="170"/>
-      <c r="AA12" s="170"/>
-      <c r="AB12" s="170"/>
-      <c r="AC12" s="170"/>
-      <c r="AD12" s="170"/>
-      <c r="AE12" s="170"/>
-      <c r="AF12" s="170"/>
-      <c r="AG12" s="170"/>
-      <c r="AH12" s="170"/>
-      <c r="AI12" s="170"/>
-      <c r="AJ12" s="171"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="172"/>
+      <c r="D12" s="172"/>
+      <c r="E12" s="172"/>
+      <c r="F12" s="172"/>
+      <c r="G12" s="172"/>
+      <c r="H12" s="172"/>
+      <c r="I12" s="172"/>
+      <c r="J12" s="172"/>
+      <c r="K12" s="172"/>
+      <c r="L12" s="172"/>
+      <c r="M12" s="172"/>
+      <c r="N12" s="172"/>
+      <c r="O12" s="172"/>
+      <c r="P12" s="172"/>
+      <c r="Q12" s="172"/>
+      <c r="R12" s="172"/>
+      <c r="S12" s="172"/>
+      <c r="T12" s="172"/>
+      <c r="U12" s="172"/>
+      <c r="V12" s="172"/>
+      <c r="W12" s="172"/>
+      <c r="X12" s="172"/>
+      <c r="Y12" s="172"/>
+      <c r="Z12" s="172"/>
+      <c r="AA12" s="172"/>
+      <c r="AB12" s="172"/>
+      <c r="AC12" s="172"/>
+      <c r="AD12" s="172"/>
+      <c r="AE12" s="172"/>
+      <c r="AF12" s="172"/>
+      <c r="AG12" s="172"/>
+      <c r="AH12" s="172"/>
+      <c r="AI12" s="172"/>
+      <c r="AJ12" s="173"/>
       <c r="AL12" s="150">
         <v>3</v>
       </c>
@@ -61284,41 +61284,41 @@
       </c>
     </row>
     <row r="13" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B13" s="169"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="170"/>
-      <c r="E13" s="170"/>
-      <c r="F13" s="170"/>
-      <c r="G13" s="170"/>
-      <c r="H13" s="170"/>
-      <c r="I13" s="170"/>
-      <c r="J13" s="170"/>
-      <c r="K13" s="170"/>
-      <c r="L13" s="170"/>
-      <c r="M13" s="170"/>
-      <c r="N13" s="170"/>
-      <c r="O13" s="170"/>
-      <c r="P13" s="170"/>
-      <c r="Q13" s="170"/>
-      <c r="R13" s="170"/>
-      <c r="S13" s="170"/>
-      <c r="T13" s="170"/>
-      <c r="U13" s="170"/>
-      <c r="V13" s="170"/>
-      <c r="W13" s="170"/>
-      <c r="X13" s="170"/>
-      <c r="Y13" s="170"/>
-      <c r="Z13" s="170"/>
-      <c r="AA13" s="170"/>
-      <c r="AB13" s="170"/>
-      <c r="AC13" s="170"/>
-      <c r="AD13" s="170"/>
-      <c r="AE13" s="170"/>
-      <c r="AF13" s="170"/>
-      <c r="AG13" s="170"/>
-      <c r="AH13" s="170"/>
-      <c r="AI13" s="170"/>
-      <c r="AJ13" s="171"/>
+      <c r="B13" s="171"/>
+      <c r="C13" s="172"/>
+      <c r="D13" s="172"/>
+      <c r="E13" s="172"/>
+      <c r="F13" s="172"/>
+      <c r="G13" s="172"/>
+      <c r="H13" s="172"/>
+      <c r="I13" s="172"/>
+      <c r="J13" s="172"/>
+      <c r="K13" s="172"/>
+      <c r="L13" s="172"/>
+      <c r="M13" s="172"/>
+      <c r="N13" s="172"/>
+      <c r="O13" s="172"/>
+      <c r="P13" s="172"/>
+      <c r="Q13" s="172"/>
+      <c r="R13" s="172"/>
+      <c r="S13" s="172"/>
+      <c r="T13" s="172"/>
+      <c r="U13" s="172"/>
+      <c r="V13" s="172"/>
+      <c r="W13" s="172"/>
+      <c r="X13" s="172"/>
+      <c r="Y13" s="172"/>
+      <c r="Z13" s="172"/>
+      <c r="AA13" s="172"/>
+      <c r="AB13" s="172"/>
+      <c r="AC13" s="172"/>
+      <c r="AD13" s="172"/>
+      <c r="AE13" s="172"/>
+      <c r="AF13" s="172"/>
+      <c r="AG13" s="172"/>
+      <c r="AH13" s="172"/>
+      <c r="AI13" s="172"/>
+      <c r="AJ13" s="173"/>
       <c r="AL13" s="150">
         <v>4</v>
       </c>
@@ -61420,41 +61420,41 @@
       </c>
     </row>
     <row r="14" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B14" s="169"/>
-      <c r="C14" s="170"/>
-      <c r="D14" s="170"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="170"/>
-      <c r="G14" s="170"/>
-      <c r="H14" s="170"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="170"/>
-      <c r="K14" s="170"/>
-      <c r="L14" s="170"/>
-      <c r="M14" s="170"/>
-      <c r="N14" s="170"/>
-      <c r="O14" s="170"/>
-      <c r="P14" s="170"/>
-      <c r="Q14" s="170"/>
-      <c r="R14" s="170"/>
-      <c r="S14" s="170"/>
-      <c r="T14" s="170"/>
-      <c r="U14" s="170"/>
-      <c r="V14" s="170"/>
-      <c r="W14" s="170"/>
-      <c r="X14" s="170"/>
-      <c r="Y14" s="170"/>
-      <c r="Z14" s="170"/>
-      <c r="AA14" s="170"/>
-      <c r="AB14" s="170"/>
-      <c r="AC14" s="170"/>
-      <c r="AD14" s="170"/>
-      <c r="AE14" s="170"/>
-      <c r="AF14" s="170"/>
-      <c r="AG14" s="170"/>
-      <c r="AH14" s="170"/>
-      <c r="AI14" s="170"/>
-      <c r="AJ14" s="171"/>
+      <c r="B14" s="171"/>
+      <c r="C14" s="172"/>
+      <c r="D14" s="172"/>
+      <c r="E14" s="172"/>
+      <c r="F14" s="172"/>
+      <c r="G14" s="172"/>
+      <c r="H14" s="172"/>
+      <c r="I14" s="172"/>
+      <c r="J14" s="172"/>
+      <c r="K14" s="172"/>
+      <c r="L14" s="172"/>
+      <c r="M14" s="172"/>
+      <c r="N14" s="172"/>
+      <c r="O14" s="172"/>
+      <c r="P14" s="172"/>
+      <c r="Q14" s="172"/>
+      <c r="R14" s="172"/>
+      <c r="S14" s="172"/>
+      <c r="T14" s="172"/>
+      <c r="U14" s="172"/>
+      <c r="V14" s="172"/>
+      <c r="W14" s="172"/>
+      <c r="X14" s="172"/>
+      <c r="Y14" s="172"/>
+      <c r="Z14" s="172"/>
+      <c r="AA14" s="172"/>
+      <c r="AB14" s="172"/>
+      <c r="AC14" s="172"/>
+      <c r="AD14" s="172"/>
+      <c r="AE14" s="172"/>
+      <c r="AF14" s="172"/>
+      <c r="AG14" s="172"/>
+      <c r="AH14" s="172"/>
+      <c r="AI14" s="172"/>
+      <c r="AJ14" s="173"/>
       <c r="AL14" s="150">
         <v>5</v>
       </c>
@@ -61556,41 +61556,41 @@
       </c>
     </row>
     <row r="15" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B15" s="169"/>
-      <c r="C15" s="170"/>
-      <c r="D15" s="170"/>
-      <c r="E15" s="170"/>
-      <c r="F15" s="170"/>
-      <c r="G15" s="170"/>
-      <c r="H15" s="170"/>
-      <c r="I15" s="170"/>
-      <c r="J15" s="170"/>
-      <c r="K15" s="170"/>
-      <c r="L15" s="170"/>
-      <c r="M15" s="170"/>
-      <c r="N15" s="170"/>
-      <c r="O15" s="170"/>
-      <c r="P15" s="170"/>
-      <c r="Q15" s="170"/>
-      <c r="R15" s="170"/>
-      <c r="S15" s="170"/>
-      <c r="T15" s="170"/>
-      <c r="U15" s="170"/>
-      <c r="V15" s="170"/>
-      <c r="W15" s="170"/>
-      <c r="X15" s="170"/>
-      <c r="Y15" s="170"/>
-      <c r="Z15" s="170"/>
-      <c r="AA15" s="170"/>
-      <c r="AB15" s="170"/>
-      <c r="AC15" s="170"/>
-      <c r="AD15" s="170"/>
-      <c r="AE15" s="170"/>
-      <c r="AF15" s="170"/>
-      <c r="AG15" s="170"/>
-      <c r="AH15" s="170"/>
-      <c r="AI15" s="170"/>
-      <c r="AJ15" s="171"/>
+      <c r="B15" s="171"/>
+      <c r="C15" s="172"/>
+      <c r="D15" s="172"/>
+      <c r="E15" s="172"/>
+      <c r="F15" s="172"/>
+      <c r="G15" s="172"/>
+      <c r="H15" s="172"/>
+      <c r="I15" s="172"/>
+      <c r="J15" s="172"/>
+      <c r="K15" s="172"/>
+      <c r="L15" s="172"/>
+      <c r="M15" s="172"/>
+      <c r="N15" s="172"/>
+      <c r="O15" s="172"/>
+      <c r="P15" s="172"/>
+      <c r="Q15" s="172"/>
+      <c r="R15" s="172"/>
+      <c r="S15" s="172"/>
+      <c r="T15" s="172"/>
+      <c r="U15" s="172"/>
+      <c r="V15" s="172"/>
+      <c r="W15" s="172"/>
+      <c r="X15" s="172"/>
+      <c r="Y15" s="172"/>
+      <c r="Z15" s="172"/>
+      <c r="AA15" s="172"/>
+      <c r="AB15" s="172"/>
+      <c r="AC15" s="172"/>
+      <c r="AD15" s="172"/>
+      <c r="AE15" s="172"/>
+      <c r="AF15" s="172"/>
+      <c r="AG15" s="172"/>
+      <c r="AH15" s="172"/>
+      <c r="AI15" s="172"/>
+      <c r="AJ15" s="173"/>
       <c r="AL15" s="150">
         <v>6</v>
       </c>
@@ -61692,41 +61692,41 @@
       </c>
     </row>
     <row r="16" spans="2:104" x14ac:dyDescent="0.3">
-      <c r="B16" s="169"/>
-      <c r="C16" s="170"/>
-      <c r="D16" s="170"/>
-      <c r="E16" s="170"/>
-      <c r="F16" s="170"/>
-      <c r="G16" s="170"/>
-      <c r="H16" s="170"/>
-      <c r="I16" s="170"/>
-      <c r="J16" s="170"/>
-      <c r="K16" s="170"/>
-      <c r="L16" s="170"/>
-      <c r="M16" s="170"/>
-      <c r="N16" s="170"/>
-      <c r="O16" s="170"/>
-      <c r="P16" s="170"/>
-      <c r="Q16" s="170"/>
-      <c r="R16" s="170"/>
-      <c r="S16" s="170"/>
-      <c r="T16" s="170"/>
-      <c r="U16" s="170"/>
-      <c r="V16" s="170"/>
-      <c r="W16" s="170"/>
-      <c r="X16" s="170"/>
-      <c r="Y16" s="170"/>
-      <c r="Z16" s="170"/>
-      <c r="AA16" s="170"/>
-      <c r="AB16" s="170"/>
-      <c r="AC16" s="170"/>
-      <c r="AD16" s="170"/>
-      <c r="AE16" s="170"/>
-      <c r="AF16" s="170"/>
-      <c r="AG16" s="170"/>
-      <c r="AH16" s="170"/>
-      <c r="AI16" s="170"/>
-      <c r="AJ16" s="171"/>
+      <c r="B16" s="171"/>
+      <c r="C16" s="172"/>
+      <c r="D16" s="172"/>
+      <c r="E16" s="172"/>
+      <c r="F16" s="172"/>
+      <c r="G16" s="172"/>
+      <c r="H16" s="172"/>
+      <c r="I16" s="172"/>
+      <c r="J16" s="172"/>
+      <c r="K16" s="172"/>
+      <c r="L16" s="172"/>
+      <c r="M16" s="172"/>
+      <c r="N16" s="172"/>
+      <c r="O16" s="172"/>
+      <c r="P16" s="172"/>
+      <c r="Q16" s="172"/>
+      <c r="R16" s="172"/>
+      <c r="S16" s="172"/>
+      <c r="T16" s="172"/>
+      <c r="U16" s="172"/>
+      <c r="V16" s="172"/>
+      <c r="W16" s="172"/>
+      <c r="X16" s="172"/>
+      <c r="Y16" s="172"/>
+      <c r="Z16" s="172"/>
+      <c r="AA16" s="172"/>
+      <c r="AB16" s="172"/>
+      <c r="AC16" s="172"/>
+      <c r="AD16" s="172"/>
+      <c r="AE16" s="172"/>
+      <c r="AF16" s="172"/>
+      <c r="AG16" s="172"/>
+      <c r="AH16" s="172"/>
+      <c r="AI16" s="172"/>
+      <c r="AJ16" s="173"/>
       <c r="AL16" s="150">
         <v>7</v>
       </c>
@@ -61828,41 +61828,41 @@
       </c>
     </row>
     <row r="17" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B17" s="169"/>
-      <c r="C17" s="170"/>
-      <c r="D17" s="170"/>
-      <c r="E17" s="170"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="170"/>
-      <c r="H17" s="170"/>
-      <c r="I17" s="170"/>
-      <c r="J17" s="170"/>
-      <c r="K17" s="170"/>
-      <c r="L17" s="170"/>
-      <c r="M17" s="170"/>
-      <c r="N17" s="170"/>
-      <c r="O17" s="170"/>
-      <c r="P17" s="170"/>
-      <c r="Q17" s="170"/>
-      <c r="R17" s="170"/>
-      <c r="S17" s="170"/>
-      <c r="T17" s="170"/>
-      <c r="U17" s="170"/>
-      <c r="V17" s="170"/>
-      <c r="W17" s="170"/>
-      <c r="X17" s="170"/>
-      <c r="Y17" s="170"/>
-      <c r="Z17" s="170"/>
-      <c r="AA17" s="170"/>
-      <c r="AB17" s="170"/>
-      <c r="AC17" s="170"/>
-      <c r="AD17" s="170"/>
-      <c r="AE17" s="170"/>
-      <c r="AF17" s="170"/>
-      <c r="AG17" s="170"/>
-      <c r="AH17" s="170"/>
-      <c r="AI17" s="170"/>
-      <c r="AJ17" s="171"/>
+      <c r="B17" s="171"/>
+      <c r="C17" s="172"/>
+      <c r="D17" s="172"/>
+      <c r="E17" s="172"/>
+      <c r="F17" s="172"/>
+      <c r="G17" s="172"/>
+      <c r="H17" s="172"/>
+      <c r="I17" s="172"/>
+      <c r="J17" s="172"/>
+      <c r="K17" s="172"/>
+      <c r="L17" s="172"/>
+      <c r="M17" s="172"/>
+      <c r="N17" s="172"/>
+      <c r="O17" s="172"/>
+      <c r="P17" s="172"/>
+      <c r="Q17" s="172"/>
+      <c r="R17" s="172"/>
+      <c r="S17" s="172"/>
+      <c r="T17" s="172"/>
+      <c r="U17" s="172"/>
+      <c r="V17" s="172"/>
+      <c r="W17" s="172"/>
+      <c r="X17" s="172"/>
+      <c r="Y17" s="172"/>
+      <c r="Z17" s="172"/>
+      <c r="AA17" s="172"/>
+      <c r="AB17" s="172"/>
+      <c r="AC17" s="172"/>
+      <c r="AD17" s="172"/>
+      <c r="AE17" s="172"/>
+      <c r="AF17" s="172"/>
+      <c r="AG17" s="172"/>
+      <c r="AH17" s="172"/>
+      <c r="AI17" s="172"/>
+      <c r="AJ17" s="173"/>
       <c r="AL17" s="150">
         <v>8</v>
       </c>
@@ -61964,41 +61964,41 @@
       </c>
     </row>
     <row r="18" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B18" s="169"/>
-      <c r="C18" s="170"/>
-      <c r="D18" s="170"/>
-      <c r="E18" s="170"/>
-      <c r="F18" s="170"/>
-      <c r="G18" s="170"/>
-      <c r="H18" s="170"/>
-      <c r="I18" s="170"/>
-      <c r="J18" s="170"/>
-      <c r="K18" s="170"/>
-      <c r="L18" s="170"/>
-      <c r="M18" s="170"/>
-      <c r="N18" s="170"/>
-      <c r="O18" s="170"/>
-      <c r="P18" s="170"/>
-      <c r="Q18" s="170"/>
-      <c r="R18" s="170"/>
-      <c r="S18" s="170"/>
-      <c r="T18" s="170"/>
-      <c r="U18" s="170"/>
-      <c r="V18" s="170"/>
-      <c r="W18" s="170"/>
-      <c r="X18" s="170"/>
-      <c r="Y18" s="170"/>
-      <c r="Z18" s="170"/>
-      <c r="AA18" s="170"/>
-      <c r="AB18" s="170"/>
-      <c r="AC18" s="170"/>
-      <c r="AD18" s="170"/>
-      <c r="AE18" s="170"/>
-      <c r="AF18" s="170"/>
-      <c r="AG18" s="170"/>
-      <c r="AH18" s="170"/>
-      <c r="AI18" s="170"/>
-      <c r="AJ18" s="171"/>
+      <c r="B18" s="171"/>
+      <c r="C18" s="172"/>
+      <c r="D18" s="172"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
+      <c r="L18" s="172"/>
+      <c r="M18" s="172"/>
+      <c r="N18" s="172"/>
+      <c r="O18" s="172"/>
+      <c r="P18" s="172"/>
+      <c r="Q18" s="172"/>
+      <c r="R18" s="172"/>
+      <c r="S18" s="172"/>
+      <c r="T18" s="172"/>
+      <c r="U18" s="172"/>
+      <c r="V18" s="172"/>
+      <c r="W18" s="172"/>
+      <c r="X18" s="172"/>
+      <c r="Y18" s="172"/>
+      <c r="Z18" s="172"/>
+      <c r="AA18" s="172"/>
+      <c r="AB18" s="172"/>
+      <c r="AC18" s="172"/>
+      <c r="AD18" s="172"/>
+      <c r="AE18" s="172"/>
+      <c r="AF18" s="172"/>
+      <c r="AG18" s="172"/>
+      <c r="AH18" s="172"/>
+      <c r="AI18" s="172"/>
+      <c r="AJ18" s="173"/>
       <c r="AL18" s="150">
         <v>9</v>
       </c>
@@ -62100,41 +62100,41 @@
       </c>
     </row>
     <row r="19" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B19" s="169"/>
-      <c r="C19" s="170"/>
-      <c r="D19" s="170"/>
-      <c r="E19" s="170"/>
-      <c r="F19" s="170"/>
-      <c r="G19" s="170"/>
-      <c r="H19" s="170"/>
-      <c r="I19" s="170"/>
-      <c r="J19" s="170"/>
-      <c r="K19" s="170"/>
-      <c r="L19" s="170"/>
-      <c r="M19" s="170"/>
-      <c r="N19" s="170"/>
-      <c r="O19" s="170"/>
-      <c r="P19" s="170"/>
-      <c r="Q19" s="170"/>
-      <c r="R19" s="170"/>
-      <c r="S19" s="170"/>
-      <c r="T19" s="170"/>
-      <c r="U19" s="170"/>
-      <c r="V19" s="170"/>
-      <c r="W19" s="170"/>
-      <c r="X19" s="170"/>
-      <c r="Y19" s="170"/>
-      <c r="Z19" s="170"/>
-      <c r="AA19" s="170"/>
-      <c r="AB19" s="170"/>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="170"/>
-      <c r="AI19" s="170"/>
-      <c r="AJ19" s="171"/>
+      <c r="B19" s="171"/>
+      <c r="C19" s="172"/>
+      <c r="D19" s="172"/>
+      <c r="E19" s="172"/>
+      <c r="F19" s="172"/>
+      <c r="G19" s="172"/>
+      <c r="H19" s="172"/>
+      <c r="I19" s="172"/>
+      <c r="J19" s="172"/>
+      <c r="K19" s="172"/>
+      <c r="L19" s="172"/>
+      <c r="M19" s="172"/>
+      <c r="N19" s="172"/>
+      <c r="O19" s="172"/>
+      <c r="P19" s="172"/>
+      <c r="Q19" s="172"/>
+      <c r="R19" s="172"/>
+      <c r="S19" s="172"/>
+      <c r="T19" s="172"/>
+      <c r="U19" s="172"/>
+      <c r="V19" s="172"/>
+      <c r="W19" s="172"/>
+      <c r="X19" s="172"/>
+      <c r="Y19" s="172"/>
+      <c r="Z19" s="172"/>
+      <c r="AA19" s="172"/>
+      <c r="AB19" s="172"/>
+      <c r="AC19" s="172"/>
+      <c r="AD19" s="172"/>
+      <c r="AE19" s="172"/>
+      <c r="AF19" s="172"/>
+      <c r="AG19" s="172"/>
+      <c r="AH19" s="172"/>
+      <c r="AI19" s="172"/>
+      <c r="AJ19" s="173"/>
       <c r="AL19" s="150">
         <v>10</v>
       </c>
@@ -62236,41 +62236,41 @@
       </c>
     </row>
     <row r="20" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B20" s="169"/>
-      <c r="C20" s="170"/>
-      <c r="D20" s="170"/>
-      <c r="E20" s="170"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170"/>
-      <c r="J20" s="170"/>
-      <c r="K20" s="170"/>
-      <c r="L20" s="170"/>
-      <c r="M20" s="170"/>
-      <c r="N20" s="170"/>
-      <c r="O20" s="170"/>
-      <c r="P20" s="170"/>
-      <c r="Q20" s="170"/>
-      <c r="R20" s="170"/>
-      <c r="S20" s="170"/>
-      <c r="T20" s="170"/>
-      <c r="U20" s="170"/>
-      <c r="V20" s="170"/>
-      <c r="W20" s="170"/>
-      <c r="X20" s="170"/>
-      <c r="Y20" s="170"/>
-      <c r="Z20" s="170"/>
-      <c r="AA20" s="170"/>
-      <c r="AB20" s="170"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="170"/>
-      <c r="AI20" s="170"/>
-      <c r="AJ20" s="171"/>
+      <c r="B20" s="171"/>
+      <c r="C20" s="172"/>
+      <c r="D20" s="172"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="172"/>
+      <c r="G20" s="172"/>
+      <c r="H20" s="172"/>
+      <c r="I20" s="172"/>
+      <c r="J20" s="172"/>
+      <c r="K20" s="172"/>
+      <c r="L20" s="172"/>
+      <c r="M20" s="172"/>
+      <c r="N20" s="172"/>
+      <c r="O20" s="172"/>
+      <c r="P20" s="172"/>
+      <c r="Q20" s="172"/>
+      <c r="R20" s="172"/>
+      <c r="S20" s="172"/>
+      <c r="T20" s="172"/>
+      <c r="U20" s="172"/>
+      <c r="V20" s="172"/>
+      <c r="W20" s="172"/>
+      <c r="X20" s="172"/>
+      <c r="Y20" s="172"/>
+      <c r="Z20" s="172"/>
+      <c r="AA20" s="172"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="172"/>
+      <c r="AD20" s="172"/>
+      <c r="AE20" s="172"/>
+      <c r="AF20" s="172"/>
+      <c r="AG20" s="172"/>
+      <c r="AH20" s="172"/>
+      <c r="AI20" s="172"/>
+      <c r="AJ20" s="173"/>
       <c r="AL20" s="150">
         <v>11</v>
       </c>
@@ -62372,41 +62372,41 @@
       </c>
     </row>
     <row r="21" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B21" s="169"/>
-      <c r="C21" s="170"/>
-      <c r="D21" s="170"/>
-      <c r="E21" s="170"/>
-      <c r="F21" s="170"/>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170"/>
-      <c r="J21" s="170"/>
-      <c r="K21" s="170"/>
-      <c r="L21" s="170"/>
-      <c r="M21" s="170"/>
-      <c r="N21" s="170"/>
-      <c r="O21" s="170"/>
-      <c r="P21" s="170"/>
-      <c r="Q21" s="170"/>
-      <c r="R21" s="170"/>
-      <c r="S21" s="170"/>
-      <c r="T21" s="170"/>
-      <c r="U21" s="170"/>
-      <c r="V21" s="170"/>
-      <c r="W21" s="170"/>
-      <c r="X21" s="170"/>
-      <c r="Y21" s="170"/>
-      <c r="Z21" s="170"/>
-      <c r="AA21" s="170"/>
-      <c r="AB21" s="170"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="170"/>
-      <c r="AI21" s="170"/>
-      <c r="AJ21" s="171"/>
+      <c r="B21" s="171"/>
+      <c r="C21" s="172"/>
+      <c r="D21" s="172"/>
+      <c r="E21" s="172"/>
+      <c r="F21" s="172"/>
+      <c r="G21" s="172"/>
+      <c r="H21" s="172"/>
+      <c r="I21" s="172"/>
+      <c r="J21" s="172"/>
+      <c r="K21" s="172"/>
+      <c r="L21" s="172"/>
+      <c r="M21" s="172"/>
+      <c r="N21" s="172"/>
+      <c r="O21" s="172"/>
+      <c r="P21" s="172"/>
+      <c r="Q21" s="172"/>
+      <c r="R21" s="172"/>
+      <c r="S21" s="172"/>
+      <c r="T21" s="172"/>
+      <c r="U21" s="172"/>
+      <c r="V21" s="172"/>
+      <c r="W21" s="172"/>
+      <c r="X21" s="172"/>
+      <c r="Y21" s="172"/>
+      <c r="Z21" s="172"/>
+      <c r="AA21" s="172"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="172"/>
+      <c r="AD21" s="172"/>
+      <c r="AE21" s="172"/>
+      <c r="AF21" s="172"/>
+      <c r="AG21" s="172"/>
+      <c r="AH21" s="172"/>
+      <c r="AI21" s="172"/>
+      <c r="AJ21" s="173"/>
       <c r="AL21" s="150">
         <v>12</v>
       </c>
@@ -62508,41 +62508,41 @@
       </c>
     </row>
     <row r="22" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B22" s="169"/>
-      <c r="C22" s="170"/>
-      <c r="D22" s="170"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="170"/>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170"/>
-      <c r="J22" s="170"/>
-      <c r="K22" s="170"/>
-      <c r="L22" s="170"/>
-      <c r="M22" s="170"/>
-      <c r="N22" s="170"/>
-      <c r="O22" s="170"/>
-      <c r="P22" s="170"/>
-      <c r="Q22" s="170"/>
-      <c r="R22" s="170"/>
-      <c r="S22" s="170"/>
-      <c r="T22" s="170"/>
-      <c r="U22" s="170"/>
-      <c r="V22" s="170"/>
-      <c r="W22" s="170"/>
-      <c r="X22" s="170"/>
-      <c r="Y22" s="170"/>
-      <c r="Z22" s="170"/>
-      <c r="AA22" s="170"/>
-      <c r="AB22" s="170"/>
-      <c r="AC22" s="170"/>
-      <c r="AD22" s="170"/>
-      <c r="AE22" s="170"/>
-      <c r="AF22" s="170"/>
-      <c r="AG22" s="170"/>
-      <c r="AH22" s="170"/>
-      <c r="AI22" s="170"/>
-      <c r="AJ22" s="171"/>
+      <c r="B22" s="171"/>
+      <c r="C22" s="172"/>
+      <c r="D22" s="172"/>
+      <c r="E22" s="172"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="172"/>
+      <c r="H22" s="172"/>
+      <c r="I22" s="172"/>
+      <c r="J22" s="172"/>
+      <c r="K22" s="172"/>
+      <c r="L22" s="172"/>
+      <c r="M22" s="172"/>
+      <c r="N22" s="172"/>
+      <c r="O22" s="172"/>
+      <c r="P22" s="172"/>
+      <c r="Q22" s="172"/>
+      <c r="R22" s="172"/>
+      <c r="S22" s="172"/>
+      <c r="T22" s="172"/>
+      <c r="U22" s="172"/>
+      <c r="V22" s="172"/>
+      <c r="W22" s="172"/>
+      <c r="X22" s="172"/>
+      <c r="Y22" s="172"/>
+      <c r="Z22" s="172"/>
+      <c r="AA22" s="172"/>
+      <c r="AB22" s="172"/>
+      <c r="AC22" s="172"/>
+      <c r="AD22" s="172"/>
+      <c r="AE22" s="172"/>
+      <c r="AF22" s="172"/>
+      <c r="AG22" s="172"/>
+      <c r="AH22" s="172"/>
+      <c r="AI22" s="172"/>
+      <c r="AJ22" s="173"/>
       <c r="AL22" s="150">
         <v>13</v>
       </c>
@@ -62644,41 +62644,41 @@
       </c>
     </row>
     <row r="23" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B23" s="169"/>
-      <c r="C23" s="170"/>
-      <c r="D23" s="170"/>
-      <c r="E23" s="170"/>
-      <c r="F23" s="170"/>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170"/>
-      <c r="J23" s="170"/>
-      <c r="K23" s="170"/>
-      <c r="L23" s="170"/>
-      <c r="M23" s="170"/>
-      <c r="N23" s="170"/>
-      <c r="O23" s="170"/>
-      <c r="P23" s="170"/>
-      <c r="Q23" s="170"/>
-      <c r="R23" s="170"/>
-      <c r="S23" s="170"/>
-      <c r="T23" s="170"/>
-      <c r="U23" s="170"/>
-      <c r="V23" s="170"/>
-      <c r="W23" s="170"/>
-      <c r="X23" s="170"/>
-      <c r="Y23" s="170"/>
-      <c r="Z23" s="170"/>
-      <c r="AA23" s="170"/>
-      <c r="AB23" s="170"/>
-      <c r="AC23" s="170"/>
-      <c r="AD23" s="170"/>
-      <c r="AE23" s="170"/>
-      <c r="AF23" s="170"/>
-      <c r="AG23" s="170"/>
-      <c r="AH23" s="170"/>
-      <c r="AI23" s="170"/>
-      <c r="AJ23" s="171"/>
+      <c r="B23" s="171"/>
+      <c r="C23" s="172"/>
+      <c r="D23" s="172"/>
+      <c r="E23" s="172"/>
+      <c r="F23" s="172"/>
+      <c r="G23" s="172"/>
+      <c r="H23" s="172"/>
+      <c r="I23" s="172"/>
+      <c r="J23" s="172"/>
+      <c r="K23" s="172"/>
+      <c r="L23" s="172"/>
+      <c r="M23" s="172"/>
+      <c r="N23" s="172"/>
+      <c r="O23" s="172"/>
+      <c r="P23" s="172"/>
+      <c r="Q23" s="172"/>
+      <c r="R23" s="172"/>
+      <c r="S23" s="172"/>
+      <c r="T23" s="172"/>
+      <c r="U23" s="172"/>
+      <c r="V23" s="172"/>
+      <c r="W23" s="172"/>
+      <c r="X23" s="172"/>
+      <c r="Y23" s="172"/>
+      <c r="Z23" s="172"/>
+      <c r="AA23" s="172"/>
+      <c r="AB23" s="172"/>
+      <c r="AC23" s="172"/>
+      <c r="AD23" s="172"/>
+      <c r="AE23" s="172"/>
+      <c r="AF23" s="172"/>
+      <c r="AG23" s="172"/>
+      <c r="AH23" s="172"/>
+      <c r="AI23" s="172"/>
+      <c r="AJ23" s="173"/>
       <c r="AL23" s="150">
         <v>14</v>
       </c>
@@ -62780,41 +62780,41 @@
       </c>
     </row>
     <row r="24" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B24" s="169"/>
-      <c r="C24" s="170"/>
-      <c r="D24" s="170"/>
-      <c r="E24" s="170"/>
-      <c r="F24" s="170"/>
-      <c r="G24" s="170"/>
-      <c r="H24" s="170"/>
-      <c r="I24" s="170"/>
-      <c r="J24" s="170"/>
-      <c r="K24" s="170"/>
-      <c r="L24" s="170"/>
-      <c r="M24" s="170"/>
-      <c r="N24" s="170"/>
-      <c r="O24" s="170"/>
-      <c r="P24" s="170"/>
-      <c r="Q24" s="170"/>
-      <c r="R24" s="170"/>
-      <c r="S24" s="170"/>
-      <c r="T24" s="170"/>
-      <c r="U24" s="170"/>
-      <c r="V24" s="170"/>
-      <c r="W24" s="170"/>
-      <c r="X24" s="170"/>
-      <c r="Y24" s="170"/>
-      <c r="Z24" s="170"/>
-      <c r="AA24" s="170"/>
-      <c r="AB24" s="170"/>
-      <c r="AC24" s="170"/>
-      <c r="AD24" s="170"/>
-      <c r="AE24" s="170"/>
-      <c r="AF24" s="170"/>
-      <c r="AG24" s="170"/>
-      <c r="AH24" s="170"/>
-      <c r="AI24" s="170"/>
-      <c r="AJ24" s="171"/>
+      <c r="B24" s="171"/>
+      <c r="C24" s="172"/>
+      <c r="D24" s="172"/>
+      <c r="E24" s="172"/>
+      <c r="F24" s="172"/>
+      <c r="G24" s="172"/>
+      <c r="H24" s="172"/>
+      <c r="I24" s="172"/>
+      <c r="J24" s="172"/>
+      <c r="K24" s="172"/>
+      <c r="L24" s="172"/>
+      <c r="M24" s="172"/>
+      <c r="N24" s="172"/>
+      <c r="O24" s="172"/>
+      <c r="P24" s="172"/>
+      <c r="Q24" s="172"/>
+      <c r="R24" s="172"/>
+      <c r="S24" s="172"/>
+      <c r="T24" s="172"/>
+      <c r="U24" s="172"/>
+      <c r="V24" s="172"/>
+      <c r="W24" s="172"/>
+      <c r="X24" s="172"/>
+      <c r="Y24" s="172"/>
+      <c r="Z24" s="172"/>
+      <c r="AA24" s="172"/>
+      <c r="AB24" s="172"/>
+      <c r="AC24" s="172"/>
+      <c r="AD24" s="172"/>
+      <c r="AE24" s="172"/>
+      <c r="AF24" s="172"/>
+      <c r="AG24" s="172"/>
+      <c r="AH24" s="172"/>
+      <c r="AI24" s="172"/>
+      <c r="AJ24" s="173"/>
       <c r="AL24" s="150">
         <v>15</v>
       </c>
@@ -62916,41 +62916,41 @@
       </c>
     </row>
     <row r="25" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B25" s="169"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="170"/>
-      <c r="E25" s="170"/>
-      <c r="F25" s="170"/>
-      <c r="G25" s="170"/>
-      <c r="H25" s="170"/>
-      <c r="I25" s="170"/>
-      <c r="J25" s="170"/>
-      <c r="K25" s="170"/>
-      <c r="L25" s="170"/>
-      <c r="M25" s="170"/>
-      <c r="N25" s="170"/>
-      <c r="O25" s="170"/>
-      <c r="P25" s="170"/>
-      <c r="Q25" s="170"/>
-      <c r="R25" s="170"/>
-      <c r="S25" s="170"/>
-      <c r="T25" s="170"/>
-      <c r="U25" s="170"/>
-      <c r="V25" s="170"/>
-      <c r="W25" s="170"/>
-      <c r="X25" s="170"/>
-      <c r="Y25" s="170"/>
-      <c r="Z25" s="170"/>
-      <c r="AA25" s="170"/>
-      <c r="AB25" s="170"/>
-      <c r="AC25" s="170"/>
-      <c r="AD25" s="170"/>
-      <c r="AE25" s="170"/>
-      <c r="AF25" s="170"/>
-      <c r="AG25" s="170"/>
-      <c r="AH25" s="170"/>
-      <c r="AI25" s="170"/>
-      <c r="AJ25" s="171"/>
+      <c r="B25" s="171"/>
+      <c r="C25" s="172"/>
+      <c r="D25" s="172"/>
+      <c r="E25" s="172"/>
+      <c r="F25" s="172"/>
+      <c r="G25" s="172"/>
+      <c r="H25" s="172"/>
+      <c r="I25" s="172"/>
+      <c r="J25" s="172"/>
+      <c r="K25" s="172"/>
+      <c r="L25" s="172"/>
+      <c r="M25" s="172"/>
+      <c r="N25" s="172"/>
+      <c r="O25" s="172"/>
+      <c r="P25" s="172"/>
+      <c r="Q25" s="172"/>
+      <c r="R25" s="172"/>
+      <c r="S25" s="172"/>
+      <c r="T25" s="172"/>
+      <c r="U25" s="172"/>
+      <c r="V25" s="172"/>
+      <c r="W25" s="172"/>
+      <c r="X25" s="172"/>
+      <c r="Y25" s="172"/>
+      <c r="Z25" s="172"/>
+      <c r="AA25" s="172"/>
+      <c r="AB25" s="172"/>
+      <c r="AC25" s="172"/>
+      <c r="AD25" s="172"/>
+      <c r="AE25" s="172"/>
+      <c r="AF25" s="172"/>
+      <c r="AG25" s="172"/>
+      <c r="AH25" s="172"/>
+      <c r="AI25" s="172"/>
+      <c r="AJ25" s="173"/>
       <c r="AL25" s="150">
         <v>16</v>
       </c>
@@ -63052,41 +63052,41 @@
       </c>
     </row>
     <row r="26" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B26" s="169"/>
-      <c r="C26" s="170"/>
-      <c r="D26" s="170"/>
-      <c r="E26" s="170"/>
-      <c r="F26" s="170"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="170"/>
-      <c r="L26" s="170"/>
-      <c r="M26" s="170"/>
-      <c r="N26" s="170"/>
-      <c r="O26" s="170"/>
-      <c r="P26" s="170"/>
-      <c r="Q26" s="170"/>
-      <c r="R26" s="170"/>
-      <c r="S26" s="170"/>
-      <c r="T26" s="170"/>
-      <c r="U26" s="170"/>
-      <c r="V26" s="170"/>
-      <c r="W26" s="170"/>
-      <c r="X26" s="170"/>
-      <c r="Y26" s="170"/>
-      <c r="Z26" s="170"/>
-      <c r="AA26" s="170"/>
-      <c r="AB26" s="170"/>
-      <c r="AC26" s="170"/>
-      <c r="AD26" s="170"/>
-      <c r="AE26" s="170"/>
-      <c r="AF26" s="170"/>
-      <c r="AG26" s="170"/>
-      <c r="AH26" s="170"/>
-      <c r="AI26" s="170"/>
-      <c r="AJ26" s="171"/>
+      <c r="B26" s="171"/>
+      <c r="C26" s="172"/>
+      <c r="D26" s="172"/>
+      <c r="E26" s="172"/>
+      <c r="F26" s="172"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="172"/>
+      <c r="I26" s="172"/>
+      <c r="J26" s="172"/>
+      <c r="K26" s="172"/>
+      <c r="L26" s="172"/>
+      <c r="M26" s="172"/>
+      <c r="N26" s="172"/>
+      <c r="O26" s="172"/>
+      <c r="P26" s="172"/>
+      <c r="Q26" s="172"/>
+      <c r="R26" s="172"/>
+      <c r="S26" s="172"/>
+      <c r="T26" s="172"/>
+      <c r="U26" s="172"/>
+      <c r="V26" s="172"/>
+      <c r="W26" s="172"/>
+      <c r="X26" s="172"/>
+      <c r="Y26" s="172"/>
+      <c r="Z26" s="172"/>
+      <c r="AA26" s="172"/>
+      <c r="AB26" s="172"/>
+      <c r="AC26" s="172"/>
+      <c r="AD26" s="172"/>
+      <c r="AE26" s="172"/>
+      <c r="AF26" s="172"/>
+      <c r="AG26" s="172"/>
+      <c r="AH26" s="172"/>
+      <c r="AI26" s="172"/>
+      <c r="AJ26" s="173"/>
       <c r="AL26" s="150">
         <v>17</v>
       </c>
@@ -63188,41 +63188,41 @@
       </c>
     </row>
     <row r="27" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B27" s="169"/>
-      <c r="C27" s="170"/>
-      <c r="D27" s="170"/>
-      <c r="E27" s="170"/>
-      <c r="F27" s="170"/>
-      <c r="G27" s="170"/>
-      <c r="H27" s="170"/>
-      <c r="I27" s="170"/>
-      <c r="J27" s="170"/>
-      <c r="K27" s="170"/>
-      <c r="L27" s="170"/>
-      <c r="M27" s="170"/>
-      <c r="N27" s="170"/>
-      <c r="O27" s="170"/>
-      <c r="P27" s="170"/>
-      <c r="Q27" s="170"/>
-      <c r="R27" s="170"/>
-      <c r="S27" s="170"/>
-      <c r="T27" s="170"/>
-      <c r="U27" s="170"/>
-      <c r="V27" s="170"/>
-      <c r="W27" s="170"/>
-      <c r="X27" s="170"/>
-      <c r="Y27" s="170"/>
-      <c r="Z27" s="170"/>
-      <c r="AA27" s="170"/>
-      <c r="AB27" s="170"/>
-      <c r="AC27" s="170"/>
-      <c r="AD27" s="170"/>
-      <c r="AE27" s="170"/>
-      <c r="AF27" s="170"/>
-      <c r="AG27" s="170"/>
-      <c r="AH27" s="170"/>
-      <c r="AI27" s="170"/>
-      <c r="AJ27" s="171"/>
+      <c r="B27" s="171"/>
+      <c r="C27" s="172"/>
+      <c r="D27" s="172"/>
+      <c r="E27" s="172"/>
+      <c r="F27" s="172"/>
+      <c r="G27" s="172"/>
+      <c r="H27" s="172"/>
+      <c r="I27" s="172"/>
+      <c r="J27" s="172"/>
+      <c r="K27" s="172"/>
+      <c r="L27" s="172"/>
+      <c r="M27" s="172"/>
+      <c r="N27" s="172"/>
+      <c r="O27" s="172"/>
+      <c r="P27" s="172"/>
+      <c r="Q27" s="172"/>
+      <c r="R27" s="172"/>
+      <c r="S27" s="172"/>
+      <c r="T27" s="172"/>
+      <c r="U27" s="172"/>
+      <c r="V27" s="172"/>
+      <c r="W27" s="172"/>
+      <c r="X27" s="172"/>
+      <c r="Y27" s="172"/>
+      <c r="Z27" s="172"/>
+      <c r="AA27" s="172"/>
+      <c r="AB27" s="172"/>
+      <c r="AC27" s="172"/>
+      <c r="AD27" s="172"/>
+      <c r="AE27" s="172"/>
+      <c r="AF27" s="172"/>
+      <c r="AG27" s="172"/>
+      <c r="AH27" s="172"/>
+      <c r="AI27" s="172"/>
+      <c r="AJ27" s="173"/>
       <c r="AL27" s="150">
         <v>18</v>
       </c>
@@ -63324,41 +63324,41 @@
       </c>
     </row>
     <row r="28" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B28" s="169"/>
-      <c r="C28" s="170"/>
-      <c r="D28" s="170"/>
-      <c r="E28" s="170"/>
-      <c r="F28" s="170"/>
-      <c r="G28" s="170"/>
-      <c r="H28" s="170"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="170"/>
-      <c r="K28" s="170"/>
-      <c r="L28" s="170"/>
-      <c r="M28" s="170"/>
-      <c r="N28" s="170"/>
-      <c r="O28" s="170"/>
-      <c r="P28" s="170"/>
-      <c r="Q28" s="170"/>
-      <c r="R28" s="170"/>
-      <c r="S28" s="170"/>
-      <c r="T28" s="170"/>
-      <c r="U28" s="170"/>
-      <c r="V28" s="170"/>
-      <c r="W28" s="170"/>
-      <c r="X28" s="170"/>
-      <c r="Y28" s="170"/>
-      <c r="Z28" s="170"/>
-      <c r="AA28" s="170"/>
-      <c r="AB28" s="170"/>
-      <c r="AC28" s="170"/>
-      <c r="AD28" s="170"/>
-      <c r="AE28" s="170"/>
-      <c r="AF28" s="170"/>
-      <c r="AG28" s="170"/>
-      <c r="AH28" s="170"/>
-      <c r="AI28" s="170"/>
-      <c r="AJ28" s="171"/>
+      <c r="B28" s="171"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="172"/>
+      <c r="E28" s="172"/>
+      <c r="F28" s="172"/>
+      <c r="G28" s="172"/>
+      <c r="H28" s="172"/>
+      <c r="I28" s="172"/>
+      <c r="J28" s="172"/>
+      <c r="K28" s="172"/>
+      <c r="L28" s="172"/>
+      <c r="M28" s="172"/>
+      <c r="N28" s="172"/>
+      <c r="O28" s="172"/>
+      <c r="P28" s="172"/>
+      <c r="Q28" s="172"/>
+      <c r="R28" s="172"/>
+      <c r="S28" s="172"/>
+      <c r="T28" s="172"/>
+      <c r="U28" s="172"/>
+      <c r="V28" s="172"/>
+      <c r="W28" s="172"/>
+      <c r="X28" s="172"/>
+      <c r="Y28" s="172"/>
+      <c r="Z28" s="172"/>
+      <c r="AA28" s="172"/>
+      <c r="AB28" s="172"/>
+      <c r="AC28" s="172"/>
+      <c r="AD28" s="172"/>
+      <c r="AE28" s="172"/>
+      <c r="AF28" s="172"/>
+      <c r="AG28" s="172"/>
+      <c r="AH28" s="172"/>
+      <c r="AI28" s="172"/>
+      <c r="AJ28" s="173"/>
       <c r="AL28" s="150">
         <v>19</v>
       </c>
@@ -63460,41 +63460,41 @@
       </c>
     </row>
     <row r="29" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B29" s="169"/>
-      <c r="C29" s="170"/>
-      <c r="D29" s="170"/>
-      <c r="E29" s="170"/>
-      <c r="F29" s="170"/>
-      <c r="G29" s="170"/>
-      <c r="H29" s="170"/>
-      <c r="I29" s="170"/>
-      <c r="J29" s="170"/>
-      <c r="K29" s="170"/>
-      <c r="L29" s="170"/>
-      <c r="M29" s="170"/>
-      <c r="N29" s="170"/>
-      <c r="O29" s="170"/>
-      <c r="P29" s="170"/>
-      <c r="Q29" s="170"/>
-      <c r="R29" s="170"/>
-      <c r="S29" s="170"/>
-      <c r="T29" s="170"/>
-      <c r="U29" s="170"/>
-      <c r="V29" s="170"/>
-      <c r="W29" s="170"/>
-      <c r="X29" s="170"/>
-      <c r="Y29" s="170"/>
-      <c r="Z29" s="170"/>
-      <c r="AA29" s="170"/>
-      <c r="AB29" s="170"/>
-      <c r="AC29" s="170"/>
-      <c r="AD29" s="170"/>
-      <c r="AE29" s="170"/>
-      <c r="AF29" s="170"/>
-      <c r="AG29" s="170"/>
-      <c r="AH29" s="170"/>
-      <c r="AI29" s="170"/>
-      <c r="AJ29" s="171"/>
+      <c r="B29" s="171"/>
+      <c r="C29" s="172"/>
+      <c r="D29" s="172"/>
+      <c r="E29" s="172"/>
+      <c r="F29" s="172"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="172"/>
+      <c r="K29" s="172"/>
+      <c r="L29" s="172"/>
+      <c r="M29" s="172"/>
+      <c r="N29" s="172"/>
+      <c r="O29" s="172"/>
+      <c r="P29" s="172"/>
+      <c r="Q29" s="172"/>
+      <c r="R29" s="172"/>
+      <c r="S29" s="172"/>
+      <c r="T29" s="172"/>
+      <c r="U29" s="172"/>
+      <c r="V29" s="172"/>
+      <c r="W29" s="172"/>
+      <c r="X29" s="172"/>
+      <c r="Y29" s="172"/>
+      <c r="Z29" s="172"/>
+      <c r="AA29" s="172"/>
+      <c r="AB29" s="172"/>
+      <c r="AC29" s="172"/>
+      <c r="AD29" s="172"/>
+      <c r="AE29" s="172"/>
+      <c r="AF29" s="172"/>
+      <c r="AG29" s="172"/>
+      <c r="AH29" s="172"/>
+      <c r="AI29" s="172"/>
+      <c r="AJ29" s="173"/>
       <c r="AL29" s="150">
         <v>20</v>
       </c>
@@ -63596,41 +63596,41 @@
       </c>
     </row>
     <row r="30" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B30" s="169"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="170"/>
-      <c r="E30" s="170"/>
-      <c r="F30" s="170"/>
-      <c r="G30" s="170"/>
-      <c r="H30" s="170"/>
-      <c r="I30" s="170"/>
-      <c r="J30" s="170"/>
-      <c r="K30" s="170"/>
-      <c r="L30" s="170"/>
-      <c r="M30" s="170"/>
-      <c r="N30" s="170"/>
-      <c r="O30" s="170"/>
-      <c r="P30" s="170"/>
-      <c r="Q30" s="170"/>
-      <c r="R30" s="170"/>
-      <c r="S30" s="170"/>
-      <c r="T30" s="170"/>
-      <c r="U30" s="170"/>
-      <c r="V30" s="170"/>
-      <c r="W30" s="170"/>
-      <c r="X30" s="170"/>
-      <c r="Y30" s="170"/>
-      <c r="Z30" s="170"/>
-      <c r="AA30" s="170"/>
-      <c r="AB30" s="170"/>
-      <c r="AC30" s="170"/>
-      <c r="AD30" s="170"/>
-      <c r="AE30" s="170"/>
-      <c r="AF30" s="170"/>
-      <c r="AG30" s="170"/>
-      <c r="AH30" s="170"/>
-      <c r="AI30" s="170"/>
-      <c r="AJ30" s="171"/>
+      <c r="B30" s="171"/>
+      <c r="C30" s="172"/>
+      <c r="D30" s="172"/>
+      <c r="E30" s="172"/>
+      <c r="F30" s="172"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="172"/>
+      <c r="K30" s="172"/>
+      <c r="L30" s="172"/>
+      <c r="M30" s="172"/>
+      <c r="N30" s="172"/>
+      <c r="O30" s="172"/>
+      <c r="P30" s="172"/>
+      <c r="Q30" s="172"/>
+      <c r="R30" s="172"/>
+      <c r="S30" s="172"/>
+      <c r="T30" s="172"/>
+      <c r="U30" s="172"/>
+      <c r="V30" s="172"/>
+      <c r="W30" s="172"/>
+      <c r="X30" s="172"/>
+      <c r="Y30" s="172"/>
+      <c r="Z30" s="172"/>
+      <c r="AA30" s="172"/>
+      <c r="AB30" s="172"/>
+      <c r="AC30" s="172"/>
+      <c r="AD30" s="172"/>
+      <c r="AE30" s="172"/>
+      <c r="AF30" s="172"/>
+      <c r="AG30" s="172"/>
+      <c r="AH30" s="172"/>
+      <c r="AI30" s="172"/>
+      <c r="AJ30" s="173"/>
       <c r="AL30" s="150">
         <v>21</v>
       </c>
@@ -63732,41 +63732,41 @@
       </c>
     </row>
     <row r="31" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B31" s="169"/>
-      <c r="C31" s="170"/>
-      <c r="D31" s="170"/>
-      <c r="E31" s="170"/>
-      <c r="F31" s="170"/>
-      <c r="G31" s="170"/>
-      <c r="H31" s="170"/>
-      <c r="I31" s="170"/>
-      <c r="J31" s="170"/>
-      <c r="K31" s="170"/>
-      <c r="L31" s="170"/>
-      <c r="M31" s="170"/>
-      <c r="N31" s="170"/>
-      <c r="O31" s="170"/>
-      <c r="P31" s="170"/>
-      <c r="Q31" s="170"/>
-      <c r="R31" s="170"/>
-      <c r="S31" s="170"/>
-      <c r="T31" s="170"/>
-      <c r="U31" s="170"/>
-      <c r="V31" s="170"/>
-      <c r="W31" s="170"/>
-      <c r="X31" s="170"/>
-      <c r="Y31" s="170"/>
-      <c r="Z31" s="170"/>
-      <c r="AA31" s="170"/>
-      <c r="AB31" s="170"/>
-      <c r="AC31" s="170"/>
-      <c r="AD31" s="170"/>
-      <c r="AE31" s="170"/>
-      <c r="AF31" s="170"/>
-      <c r="AG31" s="170"/>
-      <c r="AH31" s="170"/>
-      <c r="AI31" s="170"/>
-      <c r="AJ31" s="171"/>
+      <c r="B31" s="171"/>
+      <c r="C31" s="172"/>
+      <c r="D31" s="172"/>
+      <c r="E31" s="172"/>
+      <c r="F31" s="172"/>
+      <c r="G31" s="172"/>
+      <c r="H31" s="172"/>
+      <c r="I31" s="172"/>
+      <c r="J31" s="172"/>
+      <c r="K31" s="172"/>
+      <c r="L31" s="172"/>
+      <c r="M31" s="172"/>
+      <c r="N31" s="172"/>
+      <c r="O31" s="172"/>
+      <c r="P31" s="172"/>
+      <c r="Q31" s="172"/>
+      <c r="R31" s="172"/>
+      <c r="S31" s="172"/>
+      <c r="T31" s="172"/>
+      <c r="U31" s="172"/>
+      <c r="V31" s="172"/>
+      <c r="W31" s="172"/>
+      <c r="X31" s="172"/>
+      <c r="Y31" s="172"/>
+      <c r="Z31" s="172"/>
+      <c r="AA31" s="172"/>
+      <c r="AB31" s="172"/>
+      <c r="AC31" s="172"/>
+      <c r="AD31" s="172"/>
+      <c r="AE31" s="172"/>
+      <c r="AF31" s="172"/>
+      <c r="AG31" s="172"/>
+      <c r="AH31" s="172"/>
+      <c r="AI31" s="172"/>
+      <c r="AJ31" s="173"/>
       <c r="AL31" s="150">
         <v>22</v>
       </c>
@@ -63868,41 +63868,41 @@
       </c>
     </row>
     <row r="32" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B32" s="169"/>
-      <c r="C32" s="170"/>
-      <c r="D32" s="170"/>
-      <c r="E32" s="170"/>
-      <c r="F32" s="170"/>
-      <c r="G32" s="170"/>
-      <c r="H32" s="170"/>
-      <c r="I32" s="170"/>
-      <c r="J32" s="170"/>
-      <c r="K32" s="170"/>
-      <c r="L32" s="170"/>
-      <c r="M32" s="170"/>
-      <c r="N32" s="170"/>
-      <c r="O32" s="170"/>
-      <c r="P32" s="170"/>
-      <c r="Q32" s="170"/>
-      <c r="R32" s="170"/>
-      <c r="S32" s="170"/>
-      <c r="T32" s="170"/>
-      <c r="U32" s="170"/>
-      <c r="V32" s="170"/>
-      <c r="W32" s="170"/>
-      <c r="X32" s="170"/>
-      <c r="Y32" s="170"/>
-      <c r="Z32" s="170"/>
-      <c r="AA32" s="170"/>
-      <c r="AB32" s="170"/>
-      <c r="AC32" s="170"/>
-      <c r="AD32" s="170"/>
-      <c r="AE32" s="170"/>
-      <c r="AF32" s="170"/>
-      <c r="AG32" s="170"/>
-      <c r="AH32" s="170"/>
-      <c r="AI32" s="170"/>
-      <c r="AJ32" s="171"/>
+      <c r="B32" s="171"/>
+      <c r="C32" s="172"/>
+      <c r="D32" s="172"/>
+      <c r="E32" s="172"/>
+      <c r="F32" s="172"/>
+      <c r="G32" s="172"/>
+      <c r="H32" s="172"/>
+      <c r="I32" s="172"/>
+      <c r="J32" s="172"/>
+      <c r="K32" s="172"/>
+      <c r="L32" s="172"/>
+      <c r="M32" s="172"/>
+      <c r="N32" s="172"/>
+      <c r="O32" s="172"/>
+      <c r="P32" s="172"/>
+      <c r="Q32" s="172"/>
+      <c r="R32" s="172"/>
+      <c r="S32" s="172"/>
+      <c r="T32" s="172"/>
+      <c r="U32" s="172"/>
+      <c r="V32" s="172"/>
+      <c r="W32" s="172"/>
+      <c r="X32" s="172"/>
+      <c r="Y32" s="172"/>
+      <c r="Z32" s="172"/>
+      <c r="AA32" s="172"/>
+      <c r="AB32" s="172"/>
+      <c r="AC32" s="172"/>
+      <c r="AD32" s="172"/>
+      <c r="AE32" s="172"/>
+      <c r="AF32" s="172"/>
+      <c r="AG32" s="172"/>
+      <c r="AH32" s="172"/>
+      <c r="AI32" s="172"/>
+      <c r="AJ32" s="173"/>
       <c r="AL32" s="150">
         <v>23</v>
       </c>
@@ -64004,41 +64004,41 @@
       </c>
     </row>
     <row r="33" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B33" s="169"/>
-      <c r="C33" s="170"/>
-      <c r="D33" s="170"/>
-      <c r="E33" s="170"/>
-      <c r="F33" s="170"/>
-      <c r="G33" s="170"/>
-      <c r="H33" s="170"/>
-      <c r="I33" s="170"/>
-      <c r="J33" s="170"/>
-      <c r="K33" s="170"/>
-      <c r="L33" s="170"/>
-      <c r="M33" s="170"/>
-      <c r="N33" s="170"/>
-      <c r="O33" s="170"/>
-      <c r="P33" s="170"/>
-      <c r="Q33" s="170"/>
-      <c r="R33" s="170"/>
-      <c r="S33" s="170"/>
-      <c r="T33" s="170"/>
-      <c r="U33" s="170"/>
-      <c r="V33" s="170"/>
-      <c r="W33" s="170"/>
-      <c r="X33" s="170"/>
-      <c r="Y33" s="170"/>
-      <c r="Z33" s="170"/>
-      <c r="AA33" s="170"/>
-      <c r="AB33" s="170"/>
-      <c r="AC33" s="170"/>
-      <c r="AD33" s="170"/>
-      <c r="AE33" s="170"/>
-      <c r="AF33" s="170"/>
-      <c r="AG33" s="170"/>
-      <c r="AH33" s="170"/>
-      <c r="AI33" s="170"/>
-      <c r="AJ33" s="171"/>
+      <c r="B33" s="171"/>
+      <c r="C33" s="172"/>
+      <c r="D33" s="172"/>
+      <c r="E33" s="172"/>
+      <c r="F33" s="172"/>
+      <c r="G33" s="172"/>
+      <c r="H33" s="172"/>
+      <c r="I33" s="172"/>
+      <c r="J33" s="172"/>
+      <c r="K33" s="172"/>
+      <c r="L33" s="172"/>
+      <c r="M33" s="172"/>
+      <c r="N33" s="172"/>
+      <c r="O33" s="172"/>
+      <c r="P33" s="172"/>
+      <c r="Q33" s="172"/>
+      <c r="R33" s="172"/>
+      <c r="S33" s="172"/>
+      <c r="T33" s="172"/>
+      <c r="U33" s="172"/>
+      <c r="V33" s="172"/>
+      <c r="W33" s="172"/>
+      <c r="X33" s="172"/>
+      <c r="Y33" s="172"/>
+      <c r="Z33" s="172"/>
+      <c r="AA33" s="172"/>
+      <c r="AB33" s="172"/>
+      <c r="AC33" s="172"/>
+      <c r="AD33" s="172"/>
+      <c r="AE33" s="172"/>
+      <c r="AF33" s="172"/>
+      <c r="AG33" s="172"/>
+      <c r="AH33" s="172"/>
+      <c r="AI33" s="172"/>
+      <c r="AJ33" s="173"/>
       <c r="AL33" s="150">
         <v>24</v>
       </c>
@@ -64140,41 +64140,41 @@
       </c>
     </row>
     <row r="34" spans="2:71" x14ac:dyDescent="0.3">
-      <c r="B34" s="172"/>
-      <c r="C34" s="173"/>
-      <c r="D34" s="173"/>
-      <c r="E34" s="173"/>
-      <c r="F34" s="173"/>
-      <c r="G34" s="173"/>
-      <c r="H34" s="173"/>
-      <c r="I34" s="173"/>
-      <c r="J34" s="173"/>
-      <c r="K34" s="173"/>
-      <c r="L34" s="173"/>
-      <c r="M34" s="173"/>
-      <c r="N34" s="173"/>
-      <c r="O34" s="173"/>
-      <c r="P34" s="173"/>
-      <c r="Q34" s="173"/>
-      <c r="R34" s="173"/>
-      <c r="S34" s="173"/>
-      <c r="T34" s="173"/>
-      <c r="U34" s="173"/>
-      <c r="V34" s="173"/>
-      <c r="W34" s="173"/>
-      <c r="X34" s="173"/>
-      <c r="Y34" s="173"/>
-      <c r="Z34" s="173"/>
-      <c r="AA34" s="173"/>
-      <c r="AB34" s="173"/>
-      <c r="AC34" s="173"/>
-      <c r="AD34" s="173"/>
-      <c r="AE34" s="173"/>
-      <c r="AF34" s="173"/>
-      <c r="AG34" s="173"/>
-      <c r="AH34" s="173"/>
-      <c r="AI34" s="173"/>
-      <c r="AJ34" s="174"/>
+      <c r="B34" s="174"/>
+      <c r="C34" s="175"/>
+      <c r="D34" s="175"/>
+      <c r="E34" s="175"/>
+      <c r="F34" s="175"/>
+      <c r="G34" s="175"/>
+      <c r="H34" s="175"/>
+      <c r="I34" s="175"/>
+      <c r="J34" s="175"/>
+      <c r="K34" s="175"/>
+      <c r="L34" s="175"/>
+      <c r="M34" s="175"/>
+      <c r="N34" s="175"/>
+      <c r="O34" s="175"/>
+      <c r="P34" s="175"/>
+      <c r="Q34" s="175"/>
+      <c r="R34" s="175"/>
+      <c r="S34" s="175"/>
+      <c r="T34" s="175"/>
+      <c r="U34" s="175"/>
+      <c r="V34" s="175"/>
+      <c r="W34" s="175"/>
+      <c r="X34" s="175"/>
+      <c r="Y34" s="175"/>
+      <c r="Z34" s="175"/>
+      <c r="AA34" s="175"/>
+      <c r="AB34" s="175"/>
+      <c r="AC34" s="175"/>
+      <c r="AD34" s="175"/>
+      <c r="AE34" s="175"/>
+      <c r="AF34" s="175"/>
+      <c r="AG34" s="175"/>
+      <c r="AH34" s="175"/>
+      <c r="AI34" s="175"/>
+      <c r="AJ34" s="176"/>
       <c r="AL34" s="150">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Gráfico da última tela.
</commit_message>
<xml_diff>
--- a/doc/TemplatePlanilhaComProjetoDoUsuario.xlsx
+++ b/doc/TemplatePlanilhaComProjetoDoUsuario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448109FD-1671-46CB-835C-5566E56FCF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5046024F-7291-453E-B9DB-0297BCBEBEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="782" firstSheet="2" activeTab="2" xr2:uid="{C6048805-B876-472F-813A-7447540CBDCB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="782" firstSheet="2" activeTab="7" xr2:uid="{C6048805-B876-472F-813A-7447540CBDCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicas de Uso" sheetId="10" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <definedName name="nomeRegiaoEco">Identificação!$E$22</definedName>
     <definedName name="nomeTopografia">Identificação!$D$24</definedName>
     <definedName name="TxDsc">Parametros!$G$2</definedName>
+    <definedName name="TxPoup">FluxoCaixaModelo!$M$8</definedName>
     <definedName name="username">Identificação!$D$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -3636,9 +3637,6 @@
   </cellStyles>
   <dxfs count="65">
     <dxf>
-      <numFmt numFmtId="8" formatCode="#,##0.00;[Red]\-#,##0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
@@ -3949,6 +3947,9 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00;[Red]\-#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
@@ -53973,14 +53974,14 @@
     <dataField name="Sum of ValorEspFaixa" fld="20" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="2">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="14" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -54110,7 +54111,7 @@
     <tableColumn id="5" xr3:uid="{5198B0B0-16AB-4E0C-A7AF-746C61E2A7BF}" name="VTCustos" dataDxfId="16">
       <calculatedColumnFormula>SUMIFS(tbResumo[ValorEspFaixa],tbResumo[Faixa],tbFcFaixa[[#This Row],[Faixa]],tbResumo[Ano],tbFcFaixa[[#This Row],[ano]])*tbFcFaixa[[#This Row],[Multiplicador]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{223E4A16-FBF0-4551-9B41-20351ACAC035}" name="VTLiquido" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="0">
+    <tableColumn id="6" xr3:uid="{223E4A16-FBF0-4551-9B41-20351ACAC035}" name="VTLiquido" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>tbFcFaixa[[#This Row],[VTReceitas]]-tbFcFaixa[[#This Row],[VTCustos]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -54119,25 +54120,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8579E6BB-FC18-4413-BA32-A3626F0BC757}" name="tbDistribuicao" displayName="tbDistribuicao" ref="BU2:BY3" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12" headerRowCellStyle="Comma" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8579E6BB-FC18-4413-BA32-A3626F0BC757}" name="tbDistribuicao" displayName="tbDistribuicao" ref="BU2:BY3" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11" headerRowCellStyle="Comma" dataCellStyle="Comma">
   <autoFilter ref="BU2:BY3" xr:uid="{8579E6BB-FC18-4413-BA32-A3626F0BC757}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{97F0A431-E53A-4173-B7B6-4F327998E570}" name="Faixa" dataDxfId="11" dataCellStyle="Comma"/>
-    <tableColumn id="2" xr3:uid="{20805444-6442-4411-912E-85D698DAB74B}" name="Grupo" dataDxfId="10" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{65663903-6B14-441D-83C6-2B6C59DB8D0E}" name="Especie" dataDxfId="9" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{E5291598-5B87-4B9B-B2F0-7A1B65646F57}" name="NomeCientifico" dataDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{DF6530C5-B271-4164-9526-8AD3E616095D}" name="NrArvores" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{97F0A431-E53A-4173-B7B6-4F327998E570}" name="Faixa" dataDxfId="10" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{20805444-6442-4411-912E-85D698DAB74B}" name="Grupo" dataDxfId="9" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{65663903-6B14-441D-83C6-2B6C59DB8D0E}" name="Especie" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{E5291598-5B87-4B9B-B2F0-7A1B65646F57}" name="NomeCientifico" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{DF6530C5-B271-4164-9526-8AD3E616095D}" name="NrArvores" dataDxfId="6" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DAC085FB-F3AD-424F-8809-C741E0F91E87}" name="tbUnid" displayName="tbUnid" ref="A1:B2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DAC085FB-F3AD-424F-8809-C741E0F91E87}" name="tbUnid" displayName="tbUnid" ref="A1:B2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:B2" xr:uid="{DAC085FB-F3AD-424F-8809-C741E0F91E87}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C44199EF-5CAF-41DE-AC50-9C8ADD924820}" name="Recurso" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{AF9227DF-33D6-480D-9CB7-FD60F7BC1811}" name="Unidade" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{C44199EF-5CAF-41DE-AC50-9C8ADD924820}" name="Recurso" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{AF9227DF-33D6-480D-9CB7-FD60F7BC1811}" name="Unidade" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -57064,7 +57065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE23690A-A895-4002-97F8-748A1ADF99F4}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -58874,8 +58875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF35BF8E-2710-4D4E-B34B-677E5C2E0561}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58991,7 +58992,7 @@
         <v>#N/A</v>
       </c>
       <c r="I3" s="18" t="e">
-        <f>G3*-1</f>
+        <f>IF(A3&lt;$M$4,0,IF(A3=$M$4,$M$5,1))</f>
         <v>#N/A</v>
       </c>
       <c r="K3" s="19" t="s">
@@ -59037,7 +59038,7 @@
         <v>#N/A</v>
       </c>
       <c r="I4" s="18" t="e">
-        <f>(I3*(1+$M$8))-G4</f>
+        <f>IF(A4&lt;$M$4,0,IF(A4=$M$4,$M$5,I3*(1+$M$8)))</f>
         <v>#N/A</v>
       </c>
       <c r="K4" s="22" t="s">
@@ -59085,7 +59086,7 @@
         <v>#N/A</v>
       </c>
       <c r="I5" s="18" t="e">
-        <f>(I4*(1+M8))-G5</f>
+        <f t="shared" ref="I5:I32" si="3">IF(A5&lt;$M$4,0,IF(A5=$M$4,$M$5,I4*(1+$M$8)))</f>
         <v>#N/A</v>
       </c>
       <c r="K5" s="22" t="s">
@@ -59133,7 +59134,7 @@
         <v>#N/A</v>
       </c>
       <c r="I6" s="18" t="e">
-        <f>I5*(1+$M$8)</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="K6" s="25" t="str">
@@ -59185,7 +59186,7 @@
         <v>#N/A</v>
       </c>
       <c r="I7" s="18" t="e">
-        <f t="shared" ref="I7:I32" si="3">I6*(1+$M$8)</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Alterações no processamento batch.
</commit_message>
<xml_diff>
--- a/doc/TemplatePlanilhaComProjetoDoUsuario.xlsx
+++ b/doc/TemplatePlanilhaComProjetoDoUsuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silva\OneDrive\Área de Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5046024F-7291-453E-B9DB-0297BCBEBEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F515D1-3E62-4F66-A01A-7682E4819EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="782" firstSheet="2" activeTab="7" xr2:uid="{C6048805-B876-472F-813A-7447540CBDCB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="782" firstSheet="2" activeTab="3" xr2:uid="{C6048805-B876-472F-813A-7447540CBDCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicas de Uso" sheetId="10" r:id="rId1"/>
@@ -35,13 +35,13 @@
     <definedName name="nomeRegiaoAdm">Identificação!$E$23</definedName>
     <definedName name="nomeRegiaoEco">Identificação!$E$22</definedName>
     <definedName name="nomeTopografia">Identificação!$D$24</definedName>
-    <definedName name="TxDsc">Parametros!$G$2</definedName>
+    <definedName name="TxDsc">Parametros!$H$2</definedName>
     <definedName name="TxPoup">FluxoCaixaModelo!$M$8</definedName>
     <definedName name="username">Identificação!$D$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId13"/>
+    <pivotCache cacheId="6" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="338">
   <si>
     <t>Verde</t>
   </si>
@@ -2288,26 +2288,34 @@
   <si>
     <t>Quantidade de mudas por espécie no hectare e em que grupo cada espécie foi incluída</t>
   </si>
+  <si>
+    <t>areaFaixa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3215,29 +3223,29 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="3" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="40" fontId="4" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="40" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3252,7 +3260,7 @@
     <xf numFmtId="9" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="38" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="38" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="38" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -3262,9 +3270,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="40" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -3276,13 +3284,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="7"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3297,37 +3305,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="14" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="15" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3339,40 +3347,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="14" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="15" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3385,19 +3393,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
@@ -3405,10 +3413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3417,7 +3422,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3430,10 +3438,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3443,10 +3451,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -3483,10 +3491,10 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3501,7 +3509,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3516,7 +3524,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3531,31 +3539,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="14" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="15" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3564,19 +3572,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3606,22 +3614,22 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3637,10 +3645,10 @@
   </cellStyles>
   <dxfs count="65">
     <dxf>
-      <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -3738,7 +3746,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -3771,7 +3779,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -3806,7 +3814,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -3839,7 +3847,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -3874,7 +3882,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -3940,7 +3948,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -3949,16 +3957,16 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="8" formatCode="#,##0.00;[Red]\-#,##0.00"/>
+      <numFmt numFmtId="168" formatCode="#,##0.00;[Red]\-#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3973,7 +3981,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4000,7 +4008,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4255,7 +4263,7 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4264,7 +4272,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0000"/>
+      <numFmt numFmtId="165" formatCode="#,##0.0000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4273,7 +4281,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.00_);[Red]\(0.00\)"/>
+      <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4539,7 +4547,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5255,7 +5263,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="750736943"/>
@@ -5317,7 +5325,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="750736527"/>
@@ -5359,7 +5367,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5396,7 +5404,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -6222,13 +6230,13 @@
     <cacheField name="siglaUnidade" numFmtId="0">
       <sharedItems/>
     </cacheField>
-    <cacheField name="Preco" numFmtId="166">
+    <cacheField name="Preco" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.0999999999999999E-2" maxValue="273.079986572265"/>
     </cacheField>
-    <cacheField name="qtdRecEspFaixa" numFmtId="167">
+    <cacheField name="qtdRecEspFaixa" numFmtId="165">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="7.5500000000000003E-3" maxValue="42.673499999999997"/>
     </cacheField>
-    <cacheField name="ValorEspFaixa" numFmtId="168">
+    <cacheField name="ValorEspFaixa" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.5646620000000001E-3" maxValue="425.952"/>
     </cacheField>
   </cacheFields>
@@ -53718,7 +53726,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5F0E4673-DC4E-4FE2-BD2D-5EED45AEFA54}" name="tbDinSilvicultura" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5F0E4673-DC4E-4FE2-BD2D-5EED45AEFA54}" name="tbDinSilvicultura" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:AF23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField showAll="0"/>
@@ -53805,9 +53813,9 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField numFmtId="166" showAll="0"/>
-    <pivotField numFmtId="167" showAll="0"/>
-    <pivotField dataField="1" numFmtId="168" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" numFmtId="166" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="14"/>
@@ -54021,7 +54029,7 @@
     <tableColumn id="18" xr3:uid="{18F2E440-9E4A-44BC-8E0B-4B79F9E22535}" name="siglaUnidade" dataDxfId="45"/>
     <tableColumn id="19" xr3:uid="{A180C5EF-79CE-40F4-8816-9FD0589DBFE1}" name="Preco" dataDxfId="44"/>
     <tableColumn id="20" xr3:uid="{C2CAD173-3150-4039-9F57-2778606908D0}" name="qtdRecEspFaixa" dataDxfId="43">
-      <calculatedColumnFormula>tbSilv[[#This Row],[qtdRecurso]]*tbSilv[[#This Row],[areaOcupacao]]/10000</calculatedColumnFormula>
+      <calculatedColumnFormula>tbSilv[[#This Row],[qtdRecurso]]*IF(tbSilv[[#This Row],[Produto]]="Mel",VLOOKUP(tbSilv[[#This Row],[Faixa]],tbFaixa[],3,0),tbSilv[[#This Row],[areaOcupacao]])/10000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{62C569F1-C13A-4831-AFC3-F00D01CFB027}" name="ValorEspFaixa" dataDxfId="42">
       <calculatedColumnFormula>tbSilv[[#This Row],[qtdRecEspFaixa]]*tbSilv[[#This Row],[Preco]]</calculatedColumnFormula>
@@ -54145,11 +54153,12 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{30218212-5786-4CE3-9D48-57844C568F07}" name="tbFaixa" displayName="tbFaixa" ref="D1:E2" totalsRowShown="0">
-  <autoFilter ref="D1:E2" xr:uid="{30218212-5786-4CE3-9D48-57844C568F07}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{30218212-5786-4CE3-9D48-57844C568F07}" name="tbFaixa" displayName="tbFaixa" ref="D1:F2" totalsRowShown="0">
+  <autoFilter ref="D1:F2" xr:uid="{30218212-5786-4CE3-9D48-57844C568F07}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5225070F-A0F1-4CF3-A935-481024E497FD}" name="Faixa"/>
     <tableColumn id="2" xr3:uid="{6C69967F-8FA3-44ED-BD2A-E02C7A9899F0}" name="QtdFaixas"/>
+    <tableColumn id="3" xr3:uid="{B8AE2432-CB46-4CFA-BF32-6429D318C80B}" name="areaFaixa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -54581,10 +54590,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F50BB3C-41CB-4DEF-A3C1-020862B4D2ED}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -54594,7 +54603,7 @@
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -54607,11 +54616,14 @@
       <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="F1" t="s">
+        <v>337</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>246</v>
       </c>
@@ -54624,11 +54636,14 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="G2" s="50">
+      <c r="F2">
+        <v>2500</v>
+      </c>
+      <c r="H2" s="50">
         <v>0.12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
     </row>
   </sheetData>
@@ -57351,8 +57366,8 @@
   </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57502,7 +57517,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="T2" s="6">
-        <f>tbSilv[[#This Row],[qtdRecurso]]*tbSilv[[#This Row],[areaOcupacao]]/10000</f>
+        <f>tbSilv[[#This Row],[qtdRecurso]]*IF(tbSilv[[#This Row],[Produto]]="Mel",VLOOKUP(tbSilv[[#This Row],[Faixa]],tbFaixa[],3,0),tbSilv[[#This Row],[areaOcupacao]])/10000</f>
         <v>4.8351600000000001</v>
       </c>
       <c r="U2" s="1">
@@ -57512,7 +57527,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -58875,8 +58890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF35BF8E-2710-4D4E-B34B-677E5C2E0561}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>